<commit_message>
Update datasets with pulumi-dotnet included
</commit_message>
<xml_diff>
--- a/Datasets/Raw-Dataset_2025-04-18.xlsx
+++ b/Datasets/Raw-Dataset_2025-04-18.xlsx
@@ -2106,133 +2106,6 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/574</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Dotnet Codegen produces invalid SDKs with clashing names for valid schemas</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">### What happened?
-Dotnet Codegen can produce invalid SDKs for valid schemas which fail to build. This is an very common thing which happens in bridged providers as can be seen by the number of workarounds we've deployed over the years: https://github.com/search?q=org%3Apulumi+CSharpName&amp;type=code&amp;p=1
-Note that this is worse for Any TF providers as currently have no facility for renaming a property.
-I believe there's at least two different variants of this:
-1. When a resource has a property of the same name
-2. When a resource is named the same way as the enclosing module
-### Example
-From pulumi-gcp:
-```json
-        "gcp:accesscontextmanager/servicePerimeters:ServicePerimeters": {
-            "properties": {
-                "parent": {
-                    "type": "string",
-                },
-                "servicePerimeters": {
-                    "type": "array",
-                    "items": {
-                        "$ref": "#/types/gcp:accesscontextmanager/ServicePerimetersServicePerimeter:ServicePerimetersServicePerimeter"
-                    },
-                }
-            },
-            "required": [
-                "parent"
-            ],
-            "inputProperties": {
-                "parent": {
-                    "type": "string",
-                    "description": "The AccessPolicy this ServicePerimeter lives in.\nFormat: accessPolicies/{policy_id}\n\n\n- - -\n",
-                    "willReplaceOnChanges": true
-                },
-                "servicePerimeters": {
-                    "type": "array",
-                    "items": {
-                        "$ref": "#/types/gcp:accesscontextmanager/ServicePerimetersServicePerimeter:ServicePerimetersServicePerimeter"
-                    },
-                }
-            },
-            "requiredInputs": [
-                "parent"
-            ],
-            "stateInputs": {
-                "description": "Input properties used for looking up and filtering ServicePerimeters resources.\n",
-                "properties": {
-                    "parent": {
-                        "type": "string",
-                        "description": "The AccessPolicy this ServicePerimeter lives in.\nFormat: accessPolicies/{policy_id}\n\n\n- - -\n",
-                        "willReplaceOnChanges": true
-                    },
-                    "servicePerimeters": {
-                        "type": "array",
-                        "items": {
-                            "$ref": "#/types/gcp:accesscontextmanager/ServicePerimetersServicePerimeter:ServicePerimetersServicePerimeter"
-                        },
-                    }
-                },
-                "type": "object"
-            }
-        },
-```
-produces:
-```terminal
-cd sdk/dotnet/ &amp;&amp; dotnet build
-Restore complete (0.9s)
-  Pulumi.Gcp failed with 1 error(s) (6.4s)
-    /Users/vvm/code/pulumi-gcp/sdk/dotnet/AccessContextManager/ServicePerimeters.cs(146,82): error CS0542: 'ServicePerimeters': member names cannot be the same as their enclosing type
-Build failed with 1 error(s) in 8.7s
-make: *** [.make/build_dotnet] Error 1
-```
-### Output of `pulumi about`
--
-### Additional context
-_No response_
-### Contributing
-Vote on this issue by adding a 👍 reaction. 
-To contribute a fix for this issue, leave a comment (and link to your pull request, if you've opened one already). 
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/571</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Improve debugging experience with `DebuggerDisplayAttribute`</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">## Hello!
-&lt;!-- Please leave this section as-is, it's designed to help others in the community know how to interact with our GitHub issues. --&gt;
-- Vote on this issue by adding a 👍 reaction
-- If you want to implement this feature, comment to let us know (we'll work with you on design, scheduling, etc.)
-## Issue details
-&lt;!-- Enhancement requests are most helpful when they describe the problem you're having as well as articulating the potential solution you'd like to see built. --&gt;
-I observe that Pulumi inputs and outputs have some display issues within the vscode debugger. For example, the debugger tends to call the `ToString` method automatically when exploring variable values, which isn't too useful in this context and leads to spurious diagnostic console output.  In other words, the debugger causes unwanted side-effects.
-&lt;img width="642" alt="Image" src="https://github.com/user-attachments/assets/c07c4b1b-1a2a-4d70-b2a2-eb64de63ac95" /&gt;
-The act of expanding the variable value in the IDE causes diagnostic spew:
-```plain
- +  pulumi:pulumi:Stack dotnet-example-yaml-dev create 1 warning
-Diagnostics:
-  pulumi:pulumi:Stack (dotnet-example-yaml-dev):
-    warning: Calling [ToString] on an [Output&lt;T&gt;] is not supported.
-    To get the value of an Output&lt;T&gt; as an Output&lt;string&gt; consider:
-    1. o.Apply(v =&gt; $"prefix{v}suffix")
-    2. Output.Format($"prefix{hostname}suffix");
-    See https://www.pulumi.com/docs/concepts/inputs-outputs for more details.
-```
-### Suggestions
-There's a set of attributes in `System.Diagnostics` to control how a debugger displays a given value. For example, one may suppress certain fields, apply format strings, and use proxy types.
-See: https://learn.microsoft.com/en-us/dotnet/framework/debug-trace-profile/enhancing-debugging-with-the-debugger-display-attributes
-I would suggest we annotate the built-in types as appropriate to improve how they're displayed. For example, a resolved input could be depicted as the literal value. In the above example, `length` is simply 3 but that's heavily obscured. At minimum, we could call an internal `toString()` method that doesn't cause spew.
-### Affected area/feature
-&lt;!-- If you know the specific area where this feature request would go (e.g. Automation API, the Pulumi Service, the Terraform bridge, etc.), feel free to put that area here.  --&gt;
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/568</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[components/c#] Enum support</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Similar to https://github.com/pulumi/pulumi/pull/19072, we should support enums in C#</x:t>
-  </x:si>
-  <x:si>
     <x:t>https://github.com/pulumi/pulumi-dotnet/issues/532</x:t>
   </x:si>
   <x:si>
@@ -2251,17 +2124,6 @@
 Vote on this issue by adding a 👍 reaction. 
 To contribute a fix for this issue, leave a comment (and link to your pull request, if you've opened one already). 
 </x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/510</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Resource properties can end up null even if marked required</x:t>
-  </x:si>
-  <x:si>
-    <x:t>We discovered this while looking into https://github.com/pulumi/pulumi-dotnet/issues/456. 
-The resource property deserialiser works via reflection so can easily override nullability annotations. 
-We should fix the deserialiser to either fill in empty for null values, or mark all the output values as nullable.</x:t>
   </x:si>
   <x:si>
     <x:t>https://github.com/pulumi/pulumi-dotnet/issues/493</x:t>
@@ -2533,32 +2395,6 @@
 ```</x:t>
   </x:si>
   <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/467</x:t>
-  </x:si>
-  <x:si>
-    <x:t>auto: `Yaml` and `Java` are missing from `ProjectRuntimeName`</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/blob/654f993bc30a9e3a0e2b3166d4273fd980a05ec3/sdk/Pulumi.Automation/ProjectRuntimeName.cs#L8-L15
-This enum is missing `Yaml` and `Java`.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/448</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Add support for invoke transforms</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/446</x:t>
-  </x:si>
-  <x:si>
-    <x:t>dotnet conversions result in errors "unable to find package" because it does not set up using a relative path</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">This results in an error before SDK generation and so conversions from terraform to csharp are broken.
-Hint: The error is likely in the pulumi-language-dotnet implementation of GenerateProject which seems to check for all the dependencies to exist and if not errors.  Other languages simply generate the project and that gets filled in afterwards.  </x:t>
-  </x:si>
-  <x:si>
     <x:t>https://github.com/pulumi/pulumi-dotnet/issues/421</x:t>
   </x:si>
   <x:si>
@@ -2584,43 +2420,6 @@
 Vote on this issue by adding a 👍 reaction. 
 To contribute a fix for this issue, leave a comment (and link to your pull request, if you've opened one already). 
 </x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/409</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Calling RegisterOutput in a Component Resource is not working with Output that contains an OutputType</x:t>
-  </x:si>
-  <x:si>
-    <x:t>As per documentation we added a `RegisterOutputs()` call to the end of our component resources.
-If you have an output value like this:
-```
-    [OutputType]
-    public sealed class ComplexOutput
-    {
-        public readonly string Name;
-        [OutputConstructor]
-        private ComplexOutput(string name)
-          Name = name;
-        }
-    }
-```
-And use this in a component resource
-```
-public sealed class MyComponentResource: ComponentResource
-{
-    public MyComponentResource(string name, Args args, ComponentResourceOptions? options = null)
-        : base("myType" name, args, options)
-    {
-      Output = Output.Create(new ComplexOutput("someValue"))
-      RegisterOutputs()
-    }
-    [Output("output")]
-    public Output&lt;ComplexOutput&gt; Output { get; init; }
-}
-```
-```
-A an exception will be raised "DatacenterOutput is not a supported argument type" in Pulumi.Serialization.Serializer.SerializeAsync</x:t>
   </x:si>
   <x:si>
     <x:t>https://github.com/pulumi/pulumi-dotnet/issues/403</x:t>
@@ -2641,26 +2440,6 @@
 Vote on this issue by adding a 👍 reaction. 
 To contribute a fix for this issue, leave a comment (and link to your pull request, if you've opened one already). 
 </x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/402</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Release process can fail</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Something's wrong with the release process, just noticed we're missing the last few releases from nuget: https://www.nuget.org/packages/Pulumi/
-No 3.68 release, and the job for it failed https://github.com/pulumi/pulumi-dotnet/actions/runs/10900286299/job/30247564709. </x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/398</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Add RPCs necessary to register engine when debugging with PULUMI_DEBUG_LANGUAGES</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Blocked by pulumi#17821
-See that PR for details and examples of how this is implemented in Go/Python/Nodejs</x:t>
   </x:si>
   <x:si>
     <x:t>https://github.com/pulumi/pulumi-dotnet/issues/391</x:t>
@@ -2808,134 +2587,6 @@
     <x:t>Add a test similar to the ones added for Python, Node.js, and Go in ttps://github.com/pulumi/pulumi/pull/17489</x:t>
   </x:si>
   <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/377</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Output values do not serialize to the same objects as they deserialize from</x:t>
-  </x:si>
-  <x:si>
-    <x:t>So we may have an edge usecase that show some intressing beauvoirs for the serialiazation.
-For Context: We have a MLC c# provider that uses the sdk generator classes as the actual output objects in the components provider implementations, to be sure our output and the schema stay in sync.
-We also use c# for the consuming side with the exact same sdk.
-Now the actual issues are the generator output classes, they look like this:
-```
-    [OutputType]
-    public sealed class DatacenterOutput
-    {
-        public readonly string Name;
-        [OutputConstructor]
-        private DatacenterOutput(string name)
-          Name = name;
-        }
-    }
-}
-```
-The problem is now they get serialized like:
-```
-{ 
-   "Name": "someValue"
-}
-```
-But then the deserialization takes the names of the properties from the Output Contructors arguments names
-So the expected value is now
-```
-{
-   "name":"someValue"
-}
-```
- Since this does not match up. The client side sets all fields to null and then the programm crashes since they were not optional.
-There are now two worarounds: Adding [Output( Name = "name"] to the property or [OutputConstructorParameter("Name")] on the constructor.
-Bot both would require you to modify the generated.
-I am happy to work on a fix, but I am really unsure how/where this is actually to be fixed. So wanted to gather some feedback on this bug.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/374</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PulumiFn.Create&lt;TStack&gt;() only accepts empty constructor stacks</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">## Hello!
-- Vote on this issue by adding a 👍 reaction
-- If you want to implement this feature, comment to let us know (we'll work with you on design, scheduling, etc.)
-## Issue details
-PulumiFn.Create&lt;TStack&gt;() only works with empty Constructors.  However, I wish to implement a web service that creates a stack per user.  Thus the web app needs to pass parameters to the Stack via the constructor.  
-```
-public class MyCustomStack: Stack
-{
-    public MyCustomStack(string parameter1, string parameter2)
-    {
-      ....
-    }
-}
-var program = PulumiFn&lt;MyCustomStack&gt;("param1", "param2");
-```
-I cannot do the following as PulumiFn is marked as an internal class.
-```
-new PulumiFn&lt;MyCustomStack&gt;(() =&gt;
-            new MyCustomStack("param1", "param2"));
-```
-### Affected area/feature
-Automation API, but could also be implemented for the CLI.
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/370</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Allow customization of JsonSerializationOptions</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">## Hello!
-&lt;!-- Please leave this section as-is, it's designed to help others in the community know how to interact with our GitHub issues. --&gt;
-- Vote on this issue by adding a 👍 reaction
-- If you want to implement this feature, comment to let us know (we'll work with you on design, scheduling, etc.)
-## Issue details
-&lt;!-- Enhancement requests are most helpful when they describe the problem you're having as well as articulating the potential solution you'd like to see built. --&gt;
-Right now to deserialize configuration Pulumi use [default settings for JsonSerializer](https://github.com/pulumi/pulumi-dotnet/blob/2aa84b517a894d432fcb1200531633ed9aee0b9b/sdk/Pulumi/Config.cs#L163). That means that if someone wants to use to use different configuration then it's forced to use eg `JsonPropertyName` and others tools on each class which makes code harder to read. It would be great if there was an option to override it and provide custom `JsonSerializerOptions`.
-### Affected area/feature
-&lt;!-- If you know the specific area where this feature request would go (e.g. Automation API, the Pulumi Service, the Terraform bridge, etc.), feel free to put that area here.  --&gt;
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/366</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Wrong type for Config in ProjectSettingsModel</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">### What happened?
-There is wrong property type for `Config` in `ProjectSettingsModel`. Right now it's [string](https://github.com/pulumi/pulumi-dotnet/blob/main/sdk/Pulumi.Automation/Serialization/ProjectSettingsModel.cs#L24) while specfication assumets it's [map](https://www.pulumi.com/docs/iac/concepts/projects/project-file/#config-options).
-That cause than when I try to use LocalWorkspace automation it crash on deserialization.
-```
-(Line: 5, Col: 3, Idx: 82) - (Line: 5, Col: 3, Idx: 82): Exception during deserialization
-```
-### Example
-Code that crashes:
-```csharp
-var args = new LocalProgramArgs($"new-stack", pathToProject);
-var stack = await LocalWorkspace.CreateOrSelectStackAsync(args);
-```
-Configuration *Pulumi.yaml*:
-```yaml
-name: MyProject
-runtime: dotnet
-description: Persistence
-config: 
-  pulumi-disable-default-providers:
-  - kubernetes
-  some-setting: dev
-```
-### Output of `pulumi about`
-I'm using NuGet package Pulumi.Automation Version="3.67.1"
-### Additional context
-_No response_
-### Contributing
-Vote on this issue by adding a 👍 reaction. 
-To contribute a fix for this issue, leave a comment (and link to your pull request, if you've opened one already). 
-</x:t>
-  </x:si>
-  <x:si>
     <x:t>https://github.com/pulumi/pulumi-dotnet/issues/365</x:t>
   </x:si>
   <x:si>
@@ -3073,68 +2724,6 @@
  - [G-Research/ApiSurface](https://github.com/G-Research/ApiSurface)</x:t>
   </x:si>
   <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/323</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ImportAsync requires dotnet build to run</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">### What happened?
-When using the `WorkspaceStack.ImportAsync` Method, it currently requires building a .NET project which may not be available if the running program is an executable. The following error message is returned:
-&lt;details&gt; 
-&lt;summary&gt;Error Message&lt;/summary&gt;
-```
-Importing (SecondStack):
-    pulumi:pulumi:Stack MyProject-SecondStack  running 'dotnet build -nologo .'
-    pulumi:pulumi:Stack MyProject-SecondStack  MSBUILD : error MSB1003: Specify a project or solution file. The current working directory does not contain a project or solution file.
-    pulumi:pulumi:Stack MyProject-SecondStack  MSBUILD : error MSB1003: Specify a project or solution file. The current working directory does not contain a project or solution file.
-    pulumi:pulumi:Stack MyProject-SecondStack  1 message
-Diagnostics:
-  pulumi:pulumi:Stack (MyProject-SecondStack):
-    MSBUILD : error MSB1003: Specify a project or solution file. The current working directory does not contain a project or solution file.
-error: failed to discover plugin requirements: 'dotnet build -nologo .' exited with non-zero exit code: 1
-Unhandled exception. Pulumi.Automation.Commands.Exceptions.CommandException: code: -1
-stdout: Importing (SecondStack):
-    pulumi:pulumi:Stack MyProject-SecondStack  running 'dotnet build -nologo .'
-    pulumi:pulumi:Stack MyProject-SecondStack  MSBUILD : error MSB1003: Specify a project or solution file. The current working directory does not contain a project or solution file.
-    pulumi:pulumi:Stack MyProject-SecondStack  MSBUILD : error MSB1003: Specify a project or solution file. The current working directory does not contain a project or solution file.
-    pulumi:pulumi:Stack MyProject-SecondStack  1 message
-Diagnostics:
-  pulumi:pulumi:Stack (MyProject-SecondStack):
-    MSBUILD : error MSB1003: Specify a project or solution file. The current working directory does not contain a project or solution file.
-stderr: error: failed to discover plugin requirements: 'dotnet build -nologo .' exited with non-zero exit code: 1
-   at Pulumi.Automation.Commands.LocalPulumiCommand.RunAsyncInner(IList`1 args, String workingDir, IDictionary`2 additionalEnv, Action`1 onStandardOutput, Action`1 onStandardError, EventLogFile eventLogFile, CancellationToken cancellationToken)
-   at Pulumi.Automation.Commands.LocalPulumiCommand.RunAsync(IList`1 args, String workingDir, IDictionary`2 additionalEnv, Action`1 onStandardOutput, Action`1 onStandardError, Action`1 onEngineEvent, CancellationToken cancellationToken)
-   at Pulumi.Automation.Workspace.RunStackCommandAsync(String stackName, IList`1 args, Action`1 onStandardOutput, Action`1 onStandardError, Action`1 onEngineEvent, CancellationToken cancellationToken)
-   at Pulumi.Automation.WorkspaceStack.RunCommandAsync(IList`1 args, Action`1 onStandardOutput, Action`1 onStandardError, Action`1 onEngineEvent, CancellationToken cancellationToken)
-```
-&lt;/details&gt;
-The expectation is that it should not need to build the .NET project if it is being executed through the automation API. Speculation from the error message suggests that to import it needs to discover the plugins to use which is obtained by building the project.
-### Example
-Example to re-produce published here - https://github.com/JasonWhall/pulumi-import-bug-sample
-### Output of `pulumi about`
-CLI
-Version      3.129.0
-Go Version   go1.22.6
-Go Compiler  gc
-Host
-OS       Microsoft Windows 10 Enterprise
-Version  10.0.19045 Build 19045
-Arch     x86_64
-Backend
-Name           
-URL            file://~
-User           
-Organizations
-Token type     personal
-### Additional context
-_No response_
-### Contributing
-Vote on this issue by adding a 👍 reaction. 
-To contribute a fix for this issue, leave a comment (and link to your pull request, if you've opened one already). 
-</x:t>
-  </x:si>
-  <x:si>
     <x:t>https://github.com/pulumi/pulumi-dotnet/issues/287</x:t>
   </x:si>
   <x:si>
@@ -3180,61 +2769,6 @@
 ```
 To prevent users from hitting this error when a new version .NET is released, and to allow us to test against all of the frameworks we purportedly support (which will ~always be multiple), we should consider running Pulumi in a way lets us determine whether any of the user's installed frameworks satisfy the `TargetFramework(s)` requirement, and if so, target that framework.
 [See the conversation here](https://docs.google.com/document/d/12ZHJZNyAJS-2RRV84I0cAdaRgcuVJQ6q8hKsHjax4bw/edit?disco=AAABPWjyb9c) for additional context/discussion.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/244</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Automation API support for `pulumi-refresh --preview-only`</x:t>
-  </x:si>
-  <x:si>
-    <x:t>## Hello!
-&lt;!-- Please leave this section as-is, it's designed to help others in the community know how to interact with our GitHub issues. --&gt;
-- Vote on this issue by adding a 👍 reaction
-- If you want to implement this feature, comment to let us know (we'll work with you on design, scheduling, etc.)
-## Issue details
-Now that the CLI supports the `preview-only` flag for `pulumi refresh` (https://github.com/pulumi/pulumi/pull/15330), it would be great to have that available for the .NET Automation API. I was going to take a stab at this myself as it should be relatively straightforward, however looking into the code, the `--skip-preview` flag is hardcoded into the args: https://github.com/pulumi/pulumi-dotnet/blob/d0039a8809f5ff4ac007c02ac694594d6a26d6f7/sdk/Pulumi.Automation/WorkspaceStack.cs#L547
-I thought it best to open a discussion on how we expect this to work. 
-To give a bit of background: we currently use the Automation API to create/manage some of our microstacks, but we are unsure on the best workflow for incorporating `pulumi refresh` into this. By it's nature, the Automation API isn't always going to prompt for manual approval, hence the `--skip-preview` flag I presume, but we want to be able to manage state drift between Pulumi and our Cloud Provider (Azure).
-Now, there are certain state differences, especially in Azure, that we are happy to apply (timestamp changes to modified dates etc), but others we don't want to auto apply and at least prompt users/tooling that there has been drift. My initial thoughts were that this would be possible with the `RefreshAsync` method and the `ExpectNoChanges` flag, but with the presence of the `--skip-preview` flag, the changes **do get applied**, and _then_ Pulumi throws a `CommandException`, which is obviously too late to do anything about as the state as been updated.
-I'd be interested to hear what is the recommended workflow for state drift/applying refreshes. Is this something that we should always just be doing, no questions asked, say before or after an update? Should we always run a refresh pre-update and abort on any changes, or at least get a set of eyes on the proposed changes first? Does it make sense to run refreshes out of process, say on a schedule? It's hard to find a recommended approach for this, especially when dealing with the Automation API.
-### Affected area/feature
-Automation API</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/229</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Add the ability to delete all resources from state using the Automation-API</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">## Hello!
-&lt;!-- Please leave this section as-is, it's designed to help others in the community know how to interact with our GitHub issues. --&gt;
-- Vote on this issue by adding a 👍 reaction
-- If you want to implement this feature, comment to let us know (we'll work with you on design, scheduling, etc.)
-## Issue details
-It would be nice to have a DeleteAllAsync version of of the [DeleteAsync](https://www.pulumi.com/docs/reference/pkg/dotnet/Pulumi.Automation/Pulumi.Automation.WorkspaceStackState.html#Pulumi_Automation_WorkspaceStackState_DeleteAsync_System_String_System_Boolean_System_Threading_CancellationToken_) method.
-### Affected area/feature
-Automation API
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/204</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CollectionBuilder .NET 8</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">## Hello!
-&lt;!-- Please leave this section as-is, it's designed to help others in the community know how to interact with our GitHub issues. --&gt;
-- Vote on this issue by adding a 👍 reaction
-- If you want to implement this feature, comment to let us know (we'll work with you on design, scheduling, etc.)
-## Issue details
-.NET 8 added support for [collection expression](https://learn.microsoft.com/en-us/dotnet/csharp/language-reference/operators/collection-expressions) and also added an annotation [`CollectionBuilder`](https://learn.microsoft.com/en-us/dotnet/csharp/language-reference/operators/collection-expressions#collection-builder) I think there are many places the Pulumi .NET code could use these to improve code syntax :)
-Especially for things like GetPolicyDocuments and Statements in AWS 🤔
-### Affected area/feature
-&lt;!-- If you know the specific area where this feature request would go (e.g. Automation API, the Pulumi Service, the Terraform bridge, etc.), feel free to put that area here.  --&gt;
-</x:t>
   </x:si>
   <x:si>
     <x:t>https://github.com/pulumi/pulumi-dotnet/issues/203</x:t>
@@ -3283,51 +2817,6 @@
 ### Affected area/feature
 &lt;!-- If you know the specific area where this feature request would go (e.g. Automation API, the Pulumi Service, the Terraform bridge, etc.), feel free to put that area here.  --&gt;
 Pulumi Core</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/202</x:t>
-  </x:si>
-  <x:si>
-    <x:t>No way to register stack level transformations using a top-level async program</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">### What happened?
-see title
-### Example
-https://www.pulumi.com/docs/concepts/options/transformations/#stack-transformations
-no way to do the above with a top-level async program such as
-```
-using System.Collections.Generic;
-using Pulumi;
-return await Deployment.RunAsync(() =&gt;
-{
-   // no way to register stack transformations with this type
-   // Export outputs here
-   return new Dictionary&lt;string, object?&gt;
-   {
-      ["outputKey"] = "outputValue"
-   };
-});
-```
-### Output of `pulumi about`
-n/a
-### Additional context
-_No response_
-### Contributing
-Vote on this issue by adding a 👍 reaction. 
-To contribute a fix for this issue, leave a comment (and link to your pull request, if you've opened one already). 
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/179</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Support explicit providers for packaged components</x:t>
-  </x:si>
-  <x:si>
-    <x:t>The Node.js and Python SDKs previously lacked support for specifying an explicit provider for a packaged component. That was resolved with https://github.com/pulumi/pulumi/pull/13282.
-Does .NET have the same limitation?
-Reference: https://github.com/pulumi/pulumi/issues/11520</x:t>
   </x:si>
   <x:si>
     <x:t>https://github.com/pulumi/pulumi-dotnet/issues/177</x:t>
@@ -3413,63 +2902,6 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/171</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Resource properties named `id` are ignored</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">### What happened?
-Regardless of the id format, and even though it matches the regular expression on the error, the resource creation always returns the following error.
-```
-*error: azure-native:apimanagement:PolicyFragment resource has a problem: 'id' does not match expression '(^[\w]+$)|(^[\w][\w\-]+[\w]$)'*
-```
-The error showed initially using v1.104.0 of the Pulumi.AzureNative library. Upgrading the library to v2.3.0 did not resolve the error.
-### Expected Behavior
-The PolicyFragment resource is created.
-### Steps to reproduce
-Create a PolicyFragment resource using C# as explained in the documentation here:
-https://www.pulumi.com/registry/packages/azure-native/api-docs/apimanagement/policyfragment/#azure-native-apimanagement-policyfragment
-Not even the provided sample passes the id validation:
-```
-using System.Collections.Generic;
-using System.Linq;
-using Pulumi;
-using AzureNative = Pulumi.AzureNative;
-return await Deployment.RunAsync(() =&gt; 
-{
-    var policyFragment = new AzureNative.ApiManagement.PolicyFragment("policyFragment", new()
-    {
-        Description = "A policy fragment example",
-        Format = "xml",
-        Id = "policyFragment1",
-        ResourceGroupName = "rg1",
-        ServiceName = "apimService1",
-        Value = "&lt;fragment&gt;&lt;json-to-xml apply=\"always\" consider-accept-header=\"false\" /&gt;&lt;/fragment&gt;",
-    });
-});
-```
-### Output of `pulumi about`
-CLI
-Version      3.78.1
-Go Version   go1.20.7
-Go Compiler  gc
-Plugins
-NAME    VERSION
-dotnet  unknown
-Host
-OS       Microsoft Windows 10 Enterprise
-Version  10.0.19044 Build 19044
-Arch     x86_64
-This project is written in dotnet: executable='C:\Program Files\dotnet\dotnet.exe' version='7.0.304'
-### Additional context
-_No response_
-### Contributing
-Vote on this issue by adding a 👍 reaction. 
-To contribute a fix for this issue, leave a comment (and link to your pull request, if you've opened one already). 
-</x:t>
-  </x:si>
-  <x:si>
     <x:t>https://github.com/pulumi/pulumi-dotnet/issues/162</x:t>
   </x:si>
   <x:si>
@@ -3501,26 +2933,6 @@
 ### Affected area/feature
 &lt;!-- If you know the specific area where this feature request would go (e.g. Automation API, the Pulumi Service, the Terraform bridge, etc.), feel free to put that area here.  --&gt;
 Logging.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/151</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Support the "release" configuration when using dotnet</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">## Hello!
-&lt;!-- Please leave this section as-is, it's designed to help others in the community know how to interact with our GitHub issues. --&gt;
-- Vote on this issue by adding a 👍 reaction
-- If you want to implement this feature, comment to let us know (we'll work with you on design, scheduling, etc.)
-## Issue details
-&lt;!-- Enhancement requests are most helpful when they describe the problem you're having as well as articulating the potential solution you'd like to see built. --&gt;
-In the CLI with the dotnet sdk, when running `pulumi up` or another command, a `dotnet build` command is executed. 
-It’s always being built in debug mode (the default configuration). 
-It would be preferred to be able to run the `dotnet build` with the release configuration.
-### Affected area/feature
-&lt;!-- If you know the specific area where this feature request would go (e.g. Automation API, the Pulumi Service, the Terraform bridge, etc.), feel free to put that area here.  --&gt;
-</x:t>
   </x:si>
   <x:si>
     <x:t>https://github.com/pulumi/pulumi-dotnet/issues/140</x:t>
@@ -3576,12 +2988,6 @@
 ### Affected area/feature
 Pulumi dotnet
 </x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/136</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Support the `--exclude-protected` flag for destroy in Automation API</x:t>
   </x:si>
   <x:si>
     <x:t>https://github.com/pulumi/pulumi-dotnet/issues/134</x:t>
@@ -3691,231 +3097,6 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/133</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Consider setting PULUMI_SKIP_UPDATE_CHECK internally for Automation API</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">### What happened?
-I'm using the pulumi dotnet automation API to deploy infrastructure on demand. I'm using the callbacks `OnStandardOutput` and `OnStandardError` on the `UpAsync` method:
-```cs
-await stack.UpAsync(new UpOptions
-{
-	OnStandardError = error =&gt; Logger.Warning("Pulumi up error on VirtualMachineId {VirtualMachineId} Error: {Error}", vm.Id, error),
-	OnStandardOutput = msg =&gt; Logger.Debug("Pulumi up output on VirtualMachineId {VirtualMachineId} Message: {Message}", vm.Id, msg)
-}, token);
-```
-I'm getting output on the `OnStandardError` when pulumi is outdated:
-```
-[10:11:39 WRN] Pulumi up error on VirtualMachineId 6f5cecf3-40e5-464e-92f0-5befd240f584 Error: warning: A new version of Pulumi is available. To upgrade from version '3.60.0' to '3.61.0', run  =&gt; Application.CloudRendering.CloudProvider
-[10:11:39 WRN] Pulumi up error on VirtualMachineId 6f5cecf3-40e5-464e-92f0-5befd240f584 Error:    $ brew update &amp;&amp; brew upgrade pulumi =&gt; Application.CloudRendering.CloudProvider
-[10:11:39 WRN] Pulumi up error on VirtualMachineId 6f5cecf3-40e5-464e-92f0-5befd240f584 Error: or visit https://pulumi.com/docs/reference/install/ for manual instructions and release notes. =&gt; Application.CloudRendering.CloudProvider
-```
-### Expected Behavior
-Add option to suppress update warnings or send them on stdout instead of stderr as it is not an error.
-### Steps to reproduce
-Use the snipped above, add a stack and adjust logging.
-### Output of `pulumi about`
-CLI
-Version      3.60.0
-Go Version   go1.20.2
-Go Compiler  gc
-Host
-OS       darwin
-Version  13.3
-Arch     arm64
-Backend
-Name           pulumi.com
-URL            xxx
-User           xxx
-Organizations  xxx
-Pulumi locates its logs in xxx by default
-warning: Failed to read project: no Pulumi.yaml project file found (searching upwards from xxx). If you have not created a project yet, use `pulumi new` to do so: no project file found
-warning: Failed to get information about the current stack: no Pulumi.yaml project file found (searching upwards from xxx). If you have not created a project yet, use `pulumi new` to do so: no project file found
-warning: A new version of Pulumi is available. To upgrade from version '3.60.0' to '3.61.0', run
-   $ brew update &amp;&amp; brew upgrade pulumi
-or visit https://pulumi.com/docs/reference/install/ for manual instructions and release notes.
-### Additional context
-_No response_
-### Contributing
-Vote on this issue by adding a 👍 reaction. 
-To contribute a fix for this issue, leave a comment (and link to your pull request, if you've opened one already). 
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/126</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Pulumi Automation API throws Grpc.Core.RpcException</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">### What happened?
-I have a ASP.net core 7 project that uses the inline Pulumi automation API.
-Example:
-```cs
-var stack = await GetStackAsync(vm, cancellationToken);
-await stack.CancelAsync(token);
-await stack.RefreshAsync(cancellationToken: token);
-await stack.UpAsync(cancellationToken: token);
-```
-I use Sentry as Error tracking system. I'm getting a log of errors (16k in the last 24h) that I only partially understand. They seem benign.
-```
-Grpc.Core.RpcException: Status(StatusCode="Unavailable", Detail="Error starting gRPC call. HttpRequestException: Connection refused (127.0.0.1:37649) SocketException: Connection refused", DebugException="System.Net.Http.HttpRequestException: Connection refused (127.0.0.1:37649)
- ---&gt; System.Net.Sockets.SocketException (111): Connection refused
-   at System.Net.Sockets.Socket.AwaitableSocketAsyncEventArgs.ThrowException(SocketError error, CancellationToken cancellationToken)
-   at System.Net.Sockets.Socket.AwaitableSocketAsyncEventArgs.System.Threading.Tasks.Sources.IValueTaskSource.GetResult(Int16 token)
-   at System.Net.Sockets.Socket.&lt;ConnectAsync&gt;g__WaitForConnectWithCancellation|281_0(AwaitableSocketAsyncEventArgs saea, ValueTask connectTask, CancellationToken cancellationToken)
-   at System.Net.Http.HttpConnectionPool.ConnectToTcpHostAsync(String host, Int32 port, HttpRequestMessage initialRequest, Boolean async, CancellationToken cancellationToken)
-   --- End of inner exception stack trace ---
-   at System.Net.Http.HttpConnectionPool.ConnectToTcpHostAsync(String host, Int32 port, HttpRequestMessage initialRequest, Boolean async, CancellationToken cancellationToken)
-   at System.Net.Http.HttpConnectionPool.ConnectAsync(HttpRequestMessage request, Boolean async, CancellationToken cancellationToken)
-   at System.Net.Http.HttpConnectionPool.AddHttp2ConnectionAsync(QueueItem queueItem)
-   at System.Threading.Tasks.TaskCompletionSourceWithCancellation`1.WaitWithCancellationAsync(CancellationToken cancellationToken)
-   at System.Net.Http.HttpConnectionPool.HttpConnectionWaiter`1.WaitForConnectionAsync(Boolean async, CancellationToken requestCancellationToken)
-   at System.Net.Http.HttpConnectionPool.SendWithVersionDetectionAndRetryAsync(HttpRequestMessage request, Boolean async, Boolean doRequestAuth, CancellationToken cancellationToken)
-   at System.Net.Http.RedirectHandler.SendAsync(HttpRequestMessage request, Boolean async, CancellationToken cancellationToken)
-   at Grpc.Net.Client.Internal.GrpcCall`2.RunCall(HttpRequestMessage request, Nullable`1 timeout)")
-  ?, in async Task GrpcEngine.LogAsync(LogRequest request)
-  ?, in async Task EngineLogger.LogAsync(LogSeverity severity, string message, Resource resource, int? streamId, bool? ephemeral)
-```
-The errors are not shown in the console and they are also not caught in a try catch block. My understanding is that in https://github.com/pulumi/pulumi-dotnet/blob/26c4b096087f2cc66981139a18e7239538b9ee3b/sdk/Pulumi.Automation/WorkspaceStack.cs#L676-L779 you create a GRPC host which lets the go runtime connect to the c# runtime. Is my assumption correct? Then when the Pulumi `UpAsync` has completed the server is destroyed before the client which generates this exception.
-### Expected Behavior
-Error is not generated if Pulumi `UpAsync` completed successfully.
-### Steps to reproduce
-Create a `LocalWorkspace` and then execute `UpAsync`
-```cs
-var stackArgs = new InlineProgramArgs("instance", stackId, program);
-stackArgs.ProjectSettings!.Backend = new ProjectBackend
-{
-	Url = "backend"
-};
-var stack = await LocalWorkspace.CreateOrSelectStackAsync(stackArgs, cancellationToken);
-```
-Catching the error is the tricky part. I can only see it being caught in Sentry. Maybe there is a different API one can consume to catch those unhandled exceptions.
-### Output of `pulumi about`
-```
-pulumi about
-CLI
-Version      3.60.0
-Go Version   go1.20.2
-Go Compiler  gc
-Host
-OS       darwin
-Version  13.3
-Arch     arm64
-Backend
-Name           pulumi.com
-URL            https://app.pulumi.com/xxx
-User           klyse
-Organizations  xxx
-Pulumi locates its logs in xxx by default
-warning: Failed to read project: no Pulumi.yaml project file found (searching upwards from xxx). If you have not created a project yet, use `pulumi new` to do so: no project file found
-warning: Failed to get information about the current stack: no Pulumi.yaml project file found (searching upwards from xxx). If you have not created a project yet, use `pulumi new` to do so: no project file found
-warning: A new version of Pulumi is available. To upgrade from version '3.60.0' to '3.61.0', run
-   $ brew update &amp;&amp; brew upgrade pulumi
-or visit https://pulumi.com/docs/reference/install/ for manual instructions and release notes.
-```
-### Additional context
-_No response_
-### Contributing
-Vote on this issue by adding a 👍 reaction. 
-To contribute a fix for this issue, leave a comment (and link to your pull request, if you've opened one already). 
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/124</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Pulumi Inline Automation API process exits immediately when hitting ctrl+c</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">### What happened?
-I have a C# pulumi project that creates cloud infrastructure. I'm using the Pulumi InlineProgram automation API to do that.
-When hitting `CTRL+C` the pulumi automation process exits immediately instead of waiting for the provided cancellation token to be canceled. This means Pulumi exits without saving the state correctly and this creates issues when retrying in a later moment. Example issue:
-`Pulumi up output on VirtualMachineId xxx Message: " Note that pulumi refresh will need to be run interactively to clear pending CREATE operations."`
-Whenever the app receives `SIGTERM` my state is broken and I need to interact manually. That's okay when I use the pulumi CLI but not when I use the Automation API.
-### Expected Behavior
-Pulumi child process stays alive until the `CancellationToken` is cancelled.
-### Steps to reproduce
-Example of the up function:
-```cs
-var token = new CancellationTokenSource().Token;
-await stack.UpAsync(new UpOptions
-{
-    OnStandardError = error =&gt; Logger.Warning("Pulumi up error on VirtualMachineId {VirtualMachineId} Error: {Error}", vm.Id, error),
-    OnStandardOutput = msg =&gt; Logger.Debug("Pulumi up output on VirtualMachineId {VirtualMachineId} Message: {Message}", vm.Id, msg)
-}, token);
-```
-Then hit `CTRL+C` during the up command
-### Output of `pulumi about`
-CLI
-Version      3.60.0
-Go Version   go1.20.2
-Go Compiler  gc
-Host
-OS       darwin
-Version  13.2.1
-Arch     arm64
-Backend
-Name           pulumi.com
-URL            xxx
-User           xxx
-Organizations  xxx, xxx
-Pulumi locates its logs in xxx by default
-warning: Failed to read project: no Pulumi.yaml project file found (searching upwards from xxx). If you have not created a project yet, use `pulumi new` to do so: no project file found
-warning: Failed to get information about the current stack: no Pulumi.yaml project file found (searching upwards from /Users/klaus). If you have not created a project yet, use `pulumi new` to do so: no project file found
-### Additional context
-_No response_
-### Contributing
-Vote on this issue by adding a 👍 reaction. 
-To contribute a fix for this issue, leave a comment (and link to your pull request, if you've opened one already). 
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/122</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Setting both Parent and DependsOn to the same component causes hang</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">The following program hangs:
-```csharp
-using System.Collections.Generic;
-using Pulumi;
-return await Deployment.RunAsync(() =&gt;
-{
-   var parent = new ComponentResource("pkg:index:first", "first");
-   var child = new ComponentResource(
-      "pkg:index:second",
-      "second",
-      new ComponentResourceOptions
-      {
-         Parent = parent,
-         DependsOn = new[]{ parent},
-      }
-   );
-   // This would freeze before the fix.
-   var custom = new CustomResource(
-      "foo:bar:baz",
-      "myresource",
-      ResourceArgs.Empty,
-      new CustomResourceOptions
-      {
-         Parent = child,
-      }
-   );
-   // Export outputs here
-   return new Dictionary&lt;string, object?&gt;
-   {
-      ["outputKey"] = "outputValue"
-   };
-});
-```
-More details in https://github.com/pulumi/pulumi/issues/12032
-</x:t>
-  </x:si>
-  <x:si>
     <x:t>https://github.com/pulumi/pulumi-dotnet/issues/102</x:t>
   </x:si>
   <x:si>
@@ -3936,140 +3117,6 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/79</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[sdk/dotnet] Cloudflare record creation throws `NullReferenceException`</x:t>
-  </x:si>
-  <x:si>
-    <x:t>### What happened?
-Hello,
-This particular behavior occurs only when setting a Cloudflare record with a value from DigitalOcean reserved ip output.
-### Steps to reproduce
-1. Create a DigitalOcean droplet
-2. Create a DigitalOcean reserved IP and attach the droplet to it
-3. Create a Cloudflare record using the reserved IP
-``` csharp
-var Droplet = new DigitalOcean.Droplet(name, new DigitalOcean.DropletArgs
-{
-    Name = name,
-    Image = image,
-    Region = region,
-    Size = size,
-    GracefulShutdown = true,
-    DropletAgent = false,
-    SshKeys = { sshKey.Fingerprint },
-    VpcUuid = vpc.Id,
-    Tags = tags,
-    UserData = userData
-});
-// Reserved IP
-var ReservedIp = new DigitalOcean.ReservedIp("reserved-ip", new DigitalOcean.ReservedIpArgs
-{
-    Region = Droplet.Region,
-    DropletId = Droplet.Id.Apply(int.Parse)
-});
-var Zone = Output.Create(Cloudflare.GetZone.InvokeAsync(new Cloudflare.GetZoneArgs
-{
-    Name = "mydomain.com"
-}));
-var ApiRecord = new Cloudflare.Record("api-record", new Cloudflare.RecordArgs
-{
-    Name = "api",
-    ZoneId = Zone.Apply(x =&gt; x.Id),
-    Type = "A",
-    Value = ReservedIp.IpAddress,
-    Ttl = 3600,
-    AllowOverwrite = true
-});
-```
-Changing the value of the record to `Droplet.Ipv4Address` solves the problem.
-### Expected Behavior
-Create the Cloudflare record with the reserved ip output.
-### Actual Behavior
-An exception is thrown. Sometimes the `pulumi up` command hangs (see screenshot below) for 3 to 5 minutes before throwing the error.
-![image](https://user-images.githubusercontent.com/1000991/213114393-22ee9628-6e12-459e-af76-1e1a25b26ea8.png)
-### Exception Thrown
-```
-Diagnostics:
-  pulumi:pulumi:Stack (octopush-production):
-    error: Running program 'D:\Projects\GitHub\OctoPush-Infrastructure\src\Cloud\bin\Debug\net6.0\Cloud.dll' failed with an unhandled exception:
-    System.NullReferenceException: Object reference not set to an instance of an object.
-       at Task&lt;HashSet&lt;string&gt;&gt; Pulumi.Deployment.GetAllTransitivelyReferencedResourceUrnsAsync(HashSet&lt;Resource&gt; resources)+(Resource r) =&gt; { }
-       at bool System.Linq.Enumerable+WhereSelectEnumerableIterator&lt;TSource, TResult&gt;.MoveNext()
-       at Task&lt;TResult[]&gt; System.Threading.Tasks.Task.WhenAll&lt;TResult&gt;(IEnumerable&lt;Task&lt;TResult&gt;&gt; tasks)
-       at async Task&lt;HashSet&lt;string&gt;&gt; Pulumi.Deployment.GetAllTransitivelyReferencedResourceUrnsAsync(HashSet&lt;Resource&gt; resources)
-       at async Task&lt;PrepareResult&gt; Pulumi.Deployment.PrepareResourceAsync(string label, Resource res, bool custom, bool remote, ResourceArgs args, ResourceOptions options)
-       at async Task&lt;(string urn, string id, Struct data, ImmutableDictionary&lt;string, ImmutableHashSet&lt;Resource&gt;&gt; dependencies)&gt; Pulumi.Deployment.RegisterResourceAsync(Resource resource, bool remote, Func&lt;string, Resource&gt; newDependency, ResourceArgs args, ResourceOptions options)
-       at async Task&lt;(string urn, string id, Struct data, ImmutableDictionary&lt;string, ImmutableHashSet&lt;Resource&gt;&gt; dependencies)&gt; Pulumi.Deployment.ReadOrRegisterResourceAsync(Resource resource, bool remote, Func&lt;string, Resource&gt; newDependency, ResourceArgs args, ResourceOptions options)
-       at async Task Pulumi.Deployment.CompleteResourceAsync(Resource resource, bool remote, Func&lt;string, Resource&gt; newDependency, ResourceArgs args, ResourceOptions options, ImmutableDictionary&lt;string, IOutputCompletionSource&gt; completionSources)
-```
-### Output of `pulumi about`
-```
-CLI
-Version      3.51.1
-Go Version   go1.19.4
-Go Compiler  gc
-Plugins
-NAME          VERSION
-azure-native  1.92.0
-cloudflare    4.15.0
-digitalocean  4.16.0
-dotnet        unknown
-Host
-OS       Microsoft Windows 11 Enterprise
-Version  10.0.22000 Build 22000
-Arch     x86_64
-This project is written in dotnet: executable='C:\Program Files\dotnet\dotnet.exe' version='7.0.102'
-```
-### Additional context
-_No response_
-### Contributing
-Vote on this issue by adding a 👍 reaction. 
-To contribute a fix for this issue, leave a comment (and link to your pull request, if you've opened one already).</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/232</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Running Pulumi commands results in VS 2022 loosing references</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">### What happened?
-I have found that when using Visual Studion 2022 (full fat VS, not VS code) for writing Pulumi C# code that when you use the Pulumi CLI to run commands like up and preview, it all works fine but when you return to VS it has lost all references to the Pulumi nuget packages and everything is underlined red. Running a build from inside VS resolves the issue until the next time you run a command. 
-Not a huge issue, but annoying!
-### Steps to reproduce
-- Open a Pulumi project in Visual Studio 2022. I am using the Enterprise edition but I would assume it doesn't matter. I am also using the 64bit version.
-- Once open, go to the Pulumi CLI and run an Up or Preview command and wait for it to complete
--  Return to VS, and see that all code is underlined red and unable to find references
-- Run a build in VS and the errors will go away
-### Expected Behavior
-For the code in VS to display the same amount of errors before and after running a Pulumi command
-### Actual Behavior
-VS looses references to nuget packages and shows errors for all Pulumi code after running Pulumi commands
-### Output of `pulumi about`
-CLI
-Version      3.45.0
-Go Version   go1.19.2
-Go Compiler  gc
-Host
-OS       debian
-Version  11.3
-Arch     x86_64
-Backend
-Name           PCM-5669BL3
-URL            file://~
-User           sam
-Organizations
-Pulumi locates its logs in /tmp by default
-### Additional context
-_No response_
-### Contributing
-Vote on this issue by adding a 👍 reaction. 
-To contribute a fix for this issue, leave a comment (and link to your pull request, if you've opened one already). 
-</x:t>
-  </x:si>
-  <x:si>
     <x:t>https://github.com/pulumi/pulumi-dotnet/issues/13</x:t>
   </x:si>
   <x:si>
@@ -4078,22 +3125,6 @@
   <x:si>
     <x:t>I'm sure we used to do this, but currently our make files are not enforcing that our dotnet sdks go through formatting. We've also got public api analyzers set up which are also not being run.
 Looks like there's been a lot of unstable movement in the dotnet sdks around this area, so make sure everything is using latest sdks before trying to fix this.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/15</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Custom resource provider in Dotnet</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">## Hello!
-&lt;!-- Please leave this section as-is, it's designed to help others in the community know how to interact with our GitHub issues. --&gt;
-- Vote on this issue by adding a 👍 reaction
-- If you want to implement this feature, comment to let us know (we'll work with you on design, scheduling, etc.)
-## Issue details
-&lt;!-- Enhancement requests are most helpful when they describe the problem you're having as well as articulating the potential solution you'd like to see built. --&gt;
-We should expose an equivalent interface to the current Go SDK required to implement a custom resource provider too so we have the option to implement native providers in other languages.
-</x:t>
   </x:si>
   <x:si>
     <x:t>https://github.com/pulumi/pulumi-dotnet/issues/16</x:t>
@@ -4121,71 +3152,6 @@
 cc @rgl</x:t>
   </x:si>
   <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/17</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Allow deserialisation of Config to custom types</x:t>
-  </x:si>
-  <x:si>
-    <x:t>## Hello!
-&lt;!-- Please leave this section as-is, it's designed to help others in the community know how to interact with our GitHub issues. --&gt;
-- Vote on this issue by adding a 👍 reaction
-- If you want to implement this feature, comment to let us know (we'll work with you on design, scheduling, etc.)
-## Issue details
-Coming from the Typescript SDK, I was surprised to find that deserialisation of config to a custom type did not work. Checking the [documentation](https://www.pulumi.com/docs/intro/concepts/config/#structured-configuration), I found that deserialisation is only supported to the `System.Text.Json.JsonElement` struct, and that the config structure must be further resolved through that class. I can't see an immediate reason for this limitation when STJ supports deserialisation to arbitrary types.
-To clarify, scenarios like this should be supported but aren't:
-```csharp
-DatabaseCredentials db = new Config().RequireSecretObject&lt;DatabaseCredentials&gt;("databaseCredentials");
-```
-### Affected area/feature
-This affects the .NET SDK's core library.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/18</x:t>
-  </x:si>
-  <x:si>
-    <x:t>InputMap with null value or empty InputJson does not generate</x:t>
-  </x:si>
-  <x:si>
-    <x:t>### What happened?
-**C#**
-```InputMap map = new Dictionary&lt;string, object&gt;(new [] { KeyValuePair.Create("key", new InputJson() )})```
-```InputMap map = new Dictionary&lt;string, object&gt;(new [] { KeyValuePair.Create("key", null )})```
-**F#**
-```fsharp
-        output {
-            //identity.Id is empty for some reason
-            let! uidId = Output.Format($"/subscriptions/{subscriptionId}/resourcegroups/{rg.Name}/providers/Microsoft.ManagedIdentity/userAssignedIdentities/{identity.Name}")
-            return dict [ uidId, InputJson.op_Implicit "{}" :&gt; obj ]
-        }
-        |&gt; InputMap.op_Implicit
-```
-when passing the map to a resource input or to the stack output, it always results in `{}`
-if I explore the content of the map, the keys/values are there:
-```map.ToOutput().Apply(x =&gt; Log.Warn(x.First().Key))```
-### Steps to reproduce
-1. Create a Dictionary of string and obj
-2. Insert any string as key and null or any form of InputJson as value
-3. Convert it to a map (implicit operator)
-4. Use it in a resource or as stack output
-### Expected Behavior
-Map to be present in the output
-### Actual Behavior
-Map is empty 
-### Output of `pulumi about`
-CLI          
-Version      3.37.2
-Go Version   go1.19
-Go Compiler  gc
-### Additional context
-_No response_
-### Contributing
-Vote on this issue by adding a 👍 reaction. 
-To contribute a fix for this issue, leave a comment (and link to your pull request, if you've opened one already). 
-### Workaround
-I was able to workaround this with ```InputJson.op_Implicit(JsonDocument.Parse("{}"))``` to be able to create resources requiring an empty JSON value on a map</x:t>
-  </x:si>
-  <x:si>
     <x:t>https://github.com/pulumi/pulumi-dotnet/issues/19</x:t>
   </x:si>
   <x:si>
@@ -4195,99 +3161,6 @@
     <x:t>When using top level statements in a dotnet program (https://www.pulumi.com/blog/pulumi-targets-dotnet-6/) this makes the unit testing approach found [here](https://github.com/pulumi/examples/tree/master/testing-unit-cs) impossible.
 With top level statements, there is no user defined class which directly implements Stack.
 How should unit testing work with top level programs? Can it work with top level programs? Do we just need to document this.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/163</x:t>
-  </x:si>
-  <x:si>
-    <x:t>LogException using Pulumi.Automation in C#</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">### What happened?
-```
-Pulumi.LogException: Error occurred during logging
-Pulumi.LogException
-Error occurred during logging
-   at Pulumi.Deployment.EngineLogger.LogAsync(LogSeverity severity, String message, Resource resource, Nullable`1 streamId, Nullable`1 ephemeral)
-   at Pulumi.Deployment.Runner.LogExceptionToErrorStream(Exception exception)
-   at Pulumi.Deployment.Runner.HandleExceptionsAsync(IEnumerable`1 exceptions)
-   at Pulumi.Deployment.&lt;&gt;c__DisplayClass71_0.&lt;&lt;RunInlineAsync&gt;b__1&gt;d.MoveNext()
---- End of stack trace from previous location ---
-   at Pulumi.Automation.WorkspaceStack.UpAsync(UpOptions options, CancellationToken cancellationToken)
-   at Pulumi.Automation.WorkspaceStack.UpAsync(UpOptions options, CancellationToken cancellationToken)
-   at MediatR.Pipeline.RequestExceptionProcessorBehavior`2.Handle(TRequest request, CancellationToken cancellationToken, RequestHandlerDelegate`1 next)
-   at MediatR.Pipeline.RequestExceptionProcessorBehavior`2.Handle(TRequest request, CancellationToken cancellationToken, RequestHandlerDelegate`1 next)
-   at MediatR.Pipeline.RequestExceptionActionProcessorBehavior`2.Handle(TRequest request, CancellationToken cancellationToken, RequestHandlerDelegate`1 next)
-   at MediatR.Pipeline.RequestExceptionActionProcessorBehavior`2.Handle(TRequest request, CancellationToken cancellationToken, RequestHandlerDelegate`1 next)
-   at MediatR.Pipeline.RequestPostProcessorBehavior`2.Handle(TRequest request, CancellationToken cancellationToken, RequestHandlerDelegate`1 next)
-   at MediatR.Pipeline.RequestPreProcessorBehavior`2.Handle(TRequest request, CancellationToken cancellationToken, RequestHandlerDelegate`1 next)
---- End of stack trace from previous location ---
-   at Polly.AsyncPolicy.&lt;&gt;c__DisplayClass40_0.&lt;&lt;ImplementationAsync&gt;b__0&gt;d.MoveNext()
---- End of stack trace from previous location ---
-   at Polly.Retry.AsyncRetryEngine.ImplementationAsync[TResult](Func`3 action, Context context, CancellationToken cancellationToken, ExceptionPredicates shouldRetryExceptionPredicates, ResultPredicates`1 shouldRetryResultPredicates, Func`5 onRetryAsync, Int32 permittedRetryCount, IEnumerable`1 sleepDurationsEnumerable, Func`4 sleepDurationProvider, Boolean continueOnCapturedContext)
-   at Polly.AsyncPolicy.ExecuteAsync(Func`3 action, Context context, CancellationToken cancellationToken, Boolean continueOnCapturedContext)
-   at MediatR.Pipeline.RequestExceptionProcessorBehavior`2.Handle(TRequest request, CancellationToken cancellationToken, RequestHandlerDelegate`1 next)
-   at MediatR.Pipeline.RequestExceptionProcessorBehavior`2.Handle(TRequest request, CancellationToken cancellationToken, RequestHandlerDelegate`1 next)
-   at MediatR.Pipeline.RequestExceptionActionProcessorBehavior`2.Handle(TRequest request, CancellationToken cancellationToken, RequestHandlerDelegate`1 next)
-   at MediatR.Pipeline.RequestExceptionActionProcessorBehavior`2.Handle(TRequest request, CancellationToken cancellationToken, RequestHandlerDelegate`1 next)
-   at MediatR.Pipeline.RequestPostProcessorBehavior`2.Handle(TRequest request, CancellationToken cancellationToken, RequestHandlerDelegate`1 next)
-   at MediatR.Pipeline.RequestPreProcessorBehavior`2.Handle(TRequest request, CancellationToken cancellationToken, RequestHandlerDelegate`1 next)
-Grpc.Core.RpcException
-Status(StatusCode="Unavailable", Detail="Error starting gRPC call. HttpRequestException: Connection refused (127.0.0.1:52034) SocketException: Connection refused", DebugException="System.Net.Http.HttpRequestException: Connection refused (127.0.0.1:52034)
- ---&gt; System.Net.Sockets.SocketException (61): Connection refused
-   at System.Net.Sockets.Socket.AwaitableSocketAsyncEventArgs.System.Threading.Tasks.Sources.IValueTaskSource.GetResult(Int16 token)
-   at System.Net.Sockets.Socket.&lt;ConnectAsync&gt;g__WaitForConnectWithCancellation|277_0(AwaitableSocketAsyncEventArgs saea, ValueTask connectTask, CancellationToken cancellationToken)
-   at System.Net.Http.HttpConnectionPool.ConnectToTcpHostAsync(String host, Int32 port, HttpRequestMessage initialRequest, Boolean async, CancellationToken cancellationToken)
-   --- End of inner exception stack trace ---
-   at System.Net.Http.HttpConnectionPool.ConnectToTcpHostAsync(String host, Int32 port, HttpRequestMessage initialRequest, Boolean async, CancellationToken cancellationToken)
-   at System.Net.Http.HttpConnectionPool.ConnectAsync(HttpRequestMessage request, Boolean async, CancellationToken cancellationToken)
-   at System.Net.Http.HttpConnectionPool.AddHttp2ConnectionAsync(HttpRequestMessage request)
-   at System.Threading.Tasks.TaskCompletionSourceWithCancellation`1.WaitWithCancellationAsync(CancellationToken cancellationToken)
-   at System.Net.Http.HttpConnectionPool.GetHttp2ConnectionAsync(HttpRequestMessage request, Boolean async, CancellationToken cancellationToken)
-   at System.Net.Http.HttpConnectionPool.SendWithVersionDetectionAndRetryAsync(HttpRequestMessage request, Boolean async, Boolean doRequestAuth, CancellationToken cancellationToken)
-   at System.Net.Http.DiagnosticsHandler.SendAsyncCore(HttpRequestMessage request, Boolean async, CancellationToken cancellationToken)
-   at System.Net.Http.RedirectHandler.SendAsync(HttpRequestMessage request, Boolean async, CancellationToken cancellationToken)
-   at Grpc.Net.Client.Internal.GrpcCall`2.RunCall(HttpRequestMessage request, Nullable`1 timeout)")
-   at Pulumi.GrpcEngine.LogAsync(LogRequest request)
-   at Pulumi.Deployment.EngineLogger.LogAsync(LogSeverity severity, String message, Resource resource, Nullable`1 streamId, Nullable`1 ephemeral)
-```
-### Steps to reproduce
-Run Pulumi up via Pulumi automation. Not sure what is causing it to happen.
-### Expected Behavior
-That the command didn't fail.
-### Actual Behavior
-It failed (see above error).
-### Versions used
-```
-CLI          
-Version      3.32.1
-Go Version   go1.18.1
-Go Compiler  gc
-Plugins
-NAME    VERSION
-aws     5.4.0
-dotnet  unknown
-tls     4.4.0
-Host     
-OS       darwin
-Version  12.3.1
-Arch     arm64
-This project is written in dotnet (/usr/local/share/dotnet/dotnet v6.0.200)
-Backend        
-URL            file://~
-Organizations  
-NAME             VERSION
-Newtonsoft.Json  13.0.1
-Pulumi           3.32.1
-Pulumi.Aws       5.4.0
-Pulumi.Tls       4.4.0
-```
-### Additional context
-_No response_
-### Contributing
-Vote on this issue by adding a 👍 reaction. 
-To contribute a fix for this issue, leave a comment (and link to your pull request, if you've opened one already). 
-</x:t>
   </x:si>
   <x:si>
     <x:t>https://github.com/pulumi/pulumi-dotnet/issues/150</x:t>
@@ -4385,32 +3258,6 @@
 Fails because the parent URN is actually `"urn:pulumi:stack::project::pulumi:pulumi:Stack$test:resource:type::myres1"`.  This is not expected, as `pulumi:pulumi:Stack` is the implicit parent, and should not be included explicitly in resource URNs.</x:t>
   </x:si>
   <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/23</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[dotnet] Support serialization of anonymous objects</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Say, a resource input has the type `InputMap&lt;object&gt;` and you assign the value as
-```cs
-Value = new Dictionary&lt;string, object&gt;
-{
-    ["prometheus"] = new
-    {
-        enabled = true,
-        servicemonitor = new { enabled = true }
-    }
-},
-```
-This code will compile but will fail at serialization time:
-```
-System.AggregateException: One or more errors occurred. (&lt;&gt;f__AnonymousType11`3[[System.String, System.Private.CoreLib, Version=5.0.0.0, Culture=neutral, PublicKeyToken=7cec85d7bea7798e],[System.String, System.Private.CoreLib,
-Version=5.0.0.0, Culture=neutral, PublicKeyToken=7cec85d7bea7798e],[System.String, System.Private.CoreLib, Version=5.0.0.0, Culture=neutral, PublicKeyToken=7cec85d7bea7798e]]
-is not a supported argument type.
-```
-The case in point is a Helm Release (see https://github.com/pulumi/pulumi-kubernetes/issues/1726) although it would be useful in many places where our .NET SDK accepts an `object`, for example for ARM Template deployment in azure-native.</x:t>
-  </x:si>
-  <x:si>
     <x:t>https://github.com/pulumi/pulumi-dotnet/issues/24</x:t>
   </x:si>
   <x:si>
@@ -4439,55 +3286,6 @@
 - [ ] Reenable this test in `sdk_driver.go`. </x:t>
   </x:si>
   <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/26</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Pulumi C#/.NET hangs when previewing a program due to dependency cycles</x:t>
-  </x:si>
-  <x:si>
-    <x:t>This issue stems from cross-checking the https://github.com/pulumi/pulumi/issues/7862 problem in C#/.NET. The problem does exist.
-## Steps to reproduce
-```csharp
-using Pulumi;
-using Pulumi.Aws.S3;
-using Pulumi.Eks;
-class MyStack : Stack
-{
-    public MyStack()
-    {
-        var cluster = new Cluster("example",
-                                  new ClusterArgs()
-                                  {
-                                      VpcId = "doesntmatter",
-                                      SkipDefaultNodeGroup = true,
-                                  });
-        new Pulumi.Aws.Eks.NodeGroup(
-            "example-ng",
-            new Pulumi.Aws.Eks.NodeGroupArgs()
-            {
-                ClusterName = "example",
-                InstanceTypes = "t3.micro",
-                NodeRoleArn = cluster.InstanceRoles.Apply(xs =&gt; xs[0].Arn),
-                SubnetIds = "doesntmatter",
-                ScalingConfig = new Pulumi.Aws.Eks.Inputs.NodeGroupScalingConfigArgs()
-                {
-                    DesiredSize = 1,
-                    MaxSize = 1,
-                    MinSize = 1,
-                },
-            },
-            new Pulumi.CustomResourceOptions()
-            {
-                Parent = cluster,
-            }
-        );
-    }
-}
-```
-Expected: pulumi preview works
-Actual: pulumi preview hangs</x:t>
-  </x:si>
-  <x:si>
     <x:t>https://github.com/pulumi/pulumi-dotnet/issues/321</x:t>
   </x:si>
   <x:si>
@@ -4496,250 +3294,6 @@
   <x:si>
     <x:t>https://github.com/pulumi/pulumi/pull/7459/checks?check_run_id=3022518024#step:17:95
 The [WorkspaceStackSupportsCancel()](https://github.com/pulumi/pulumi/blob/22669d70fc1ab4acfe214776a602bc8b7a72e62a/sdk/dotnet/Pulumi.Automation.Tests/LocalWorkspaceTests.cs#L1434) is flakey and consistently breaks builds so it has been turned off.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/28</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Add Helper Method to allow Output "All" to Support .NET Dictionary Types</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">&lt;!-- Enhancement requests are most helpful when they describe the problem you're having as well as articulating the potential solution you'd like to see built. --&gt;
-Output.All() does not support dictionary types, as it does enumerable types. It would be useful to have a helper method to transform a Dictionary into an Output type, much like Output.All() does for enumerable types.
-```csharp
-var dictionary = new Dictionary&lt;string, Output&lt;string&gt;&gt;();
-var list = new List&lt;Output&lt;string&gt;&gt;();
-for (var i = 0; i &lt; 3; i++)
-{
-    var key = $"bucket-{i}";
-    var bucket = new Bucket(key);
-    list.Add(bucket.Id);
-    dictionary.Add(DateTime.Now.Ticks.ToString(), bucket.Id);
-}
-// All accepts enumerable types
-BucketIds = Output.All(list);
-// All does not have a helper method for dictionaries
-// DOES NOT COMPILE
-BucketData = Output.All(dictionary);
-```
-Currently, this can be supported by passing the Dictionary's "Values" to Output.All(), however, one then has to join the dictionary Keys and the output values into an ImmutableDictionary before exiting the program. 
-Possibly, a new All() helper method could be created separate the Keys and Values of the incoming dictionary, create OutputData for the Values, specifically, and join Keys and new Values into a new dictionary before returning to the caller?
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/29</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[dotnet] Let the Pulumi CLI search for the binary and then for the .csproj</x:t>
-  </x:si>
-  <x:si>
-    <x:t>According to the [documentation](https://www.pulumi.com/docs/reference/pulumi-yaml/#:~:text=.NET%3A%20A%20string%20that%20specifies%20the%20path%20of%20a%20pre-built%20.NET%20assembly.%20If%20not%20specified%2C%20a%20.NET%20project%20in%20%24CWD%20will%20be%20invoked%20via%20dotnet%20run.), 
-&gt; binary: applies to Go and .NET projects only
-&gt; - .NET: A string that specifies the path of a pre-built .NET assembly. If not specified, a .NET project in $CWD will be invoked via dotnet run.
-Can we let the CLI search for the .csproj after it doesn't find a .dll?
-If I understand the code correctly, it should be done somewhere here: https://github.com/pulumi/pulumi/blob/a41ed7594272adcbc5494ddc1f4ed08e64a093c4/sdk/dotnet/cmd/pulumi-language-dotnet/main.go#L66-L81
-I have the following scenario:
-`Pulumi.yaml.dev`
-```
-name: Infra
-runtime:
-    name: dotnet
-    options:
-        binary: MyProject.dll
-description: A minimal Azure Native C# Pulumi program
-```
-I use the binary in the my CI/CD pipeline and it works as expected. However, when I try to run the project locally with `pulumi preview` it can't find the .dll
-```
-Diagnostics:
-  pulumi:pulumi:Stack (Infra-dev):
-    Could not execute because the specified command or file was not found.
-    Possible reasons for this include:
-      * You misspelled a built-in dotnet command.
-      * You intended to execute a .NET program, but dotnet-MyProject.dll does not exist.
-      * You intended to run a global tool, but a dotnet-prefixed executable with this name could not be found on the PATH.
-    error: an unhandled error occurred: Program exited with non-zero exit code: 1
-```
-Which is expected, on my local machine the .dll is somewhere in `bin/(Debug/Release)/net5.0`.
-The only way to make it work is either running `pulumi preview --cwd="bin/Debug/net5.0"` or commenting out the options as suggested [here](https://github.com/pulumi/pulumi/issues/5334#issuecomment-691742333). Both are a bit inconvenient.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/31</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Unable to specify enumerated properties as strings</x:t>
-  </x:si>
-  <x:si>
-    <x:t>With AzureNextGen/DotNet I could use string instead of enumeration values for properties such as the Tier and Name when creating a Service Bus Namespace
-```
-Sku = new AzureNative.ServiceBus.Inputs.SBSkuArgs
-{
-    Name =  "Standard",
-    Tier = "Standard",
-}
-```
-This was handy when pulling these values from a config yaml file.
-With AzureNative I am unable to do this.  If I try to use a string variable here I get the following error
-*Cannot implicitly convert type 'string' to 'Pulumi.Input&lt;Pulumi.AzureNative.ServiceBus.SkuName&gt;'*
-If the string value is stored in a variable called configName I have to use the following ugly code
-```
-Sku = new AzureNative.ServiceBus.Inputs.SBSkuArgs
-{
-    Name =  (SkuTier)(typeof(SkuTier).GetProperty(configName )?.GetValue(null))!,
-} 
-```
-Can we please allow these areas to accept string inputs again?
-## Steps to reproduce
-Try to create a new AzureNative ServiceBusNamespace and specify the Name or Tier as a string e.g. 
-Name = "Standard",
-Thanks
-Alan</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/32</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Urn property left null when a Resource subclass accidentally redefines it</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">If a class inherits from `Resource` and defines a property called `Urn`, we start getting NullPointer exceptions from core code as the `Resource.Urn` property is left undefined.
-From C# language point of view, the `Urn` property is non-virtual already, and *cannot* be overridden by subclasses. It cannot be marked `sealed` to throw a compiler error when users override it accidentally. 
-However, it appears that Pulumi SDK does not set the `Urn` property using regular C# statically checked assignment, but instead uses reflection. I have not narrowed it down with full confidence but I think this might be happening in `OutputCompletionSource.InitializeOutputs`. Therefore, this reflection code emulates virtual properties, and ends up assigning the wrong property.
-It is possible that the name conflict is also an issue in some RPC protocol if it contends for the same slot on a serializer object, and cannot be fixed simply be editing the C# code.
-So stepping back, a fix here would:
-- either allow properties called Urn to work as expected on resources
-- give clear feedback to the user that they cannot define a property called Urn and need to rename it (and we want this feedback on all auto-generated providers also)
-## Steps to reproduce
-See https://github.com/pulumi/examples/issues/1017
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/33</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Pulumi C# v3.2.1 is running Output.Apply in preview</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">When running `pulumi up` with Azure Native I'm getting a `ResourceNotFound` error, but it's just a preview so shouldn't be executing the code that's causing the error.
-## Expected behavior
-I expect for a preview that the Output.Apply code block is not executed, [as per the documentation](https://www.pulumi.com/docs/intro/concepts/inputs-outputs/#apply).
-## Current behavior
-The Apply code block is being executed.
-## Steps to reproduce
-```
-var functionApp = new WebApp("functionsApp", new WebAppArgs
-  {
-      ResourceGroupName = resGroup.Name,
-      Name = "fn-uat",
-      ServerFarmId = plan.Id,
-      Kind = "functionapp",
-  });
-this.FunctionAppKey = Output.Tuple(functionApp.Name, resGroup.Name, Output.CreateSecret("")).Apply(
-    t =&gt; ListWebAppHostKeys.InvokeAsync(new ListWebAppHostKeysArgs
-    {
-        Name = t.Item1,
-        ResourceGroupName = t.Item2,
-    })).Apply(result =&gt; result.MasterKey);
-```
-## Context (Environment)
-This only reared it's head as I'm deploying a new environment for the first time. Here's the redacted log.
-```
-Previewing update (uat)
-View Live: https://app.pulumi.com/...
-     Type                                                   Name                      Plan       Info
-     pulumi:pulumi:Stack                                    integrations-uat      1 error; 1 message
- ~   ├─ azure-native:web:AppServicePlan                     plan                      update     [diff: ~sku]
- +   ├─ azure-native:apimanagement:ApiManagementService     apiService                create     
- +   ├─ azure-native:sql:FirewallRule                       sqlDbFirewallAllowAzure   create     
- +   ├─ azure-native:sql:Database                           sqlDb                     create     
- +   ├─ azure-native:servicebus:Queue                       emailQueue                create     
- +   ├─ azure-native:servicebus:NamespaceAuthorizationRule  busRuleSendListen         create     
- +   ├─ azure-native:apimanagement:NamedValue               partnerPortalAppIdValue   create     
- +   ├─ azure-native:apimanagement:NamedValue               openIdConfigUrlValue      create     
- +   ├─ azure-native:apimanagement:ApiVersionSet            partnerVersionSet         create     
- +   ├─ azure-native:apimanagement:User                     partnerUser               create     
- +   ├─ azure-native:apimanagement:Logger                   apiLogger                 create     
- +   ├─ azure-native:apimanagement:Product                  partnerProduct            create     
- +   ├─ azure-native:apimanagement:Subscription             subscription              create     
- +   ├─ azure-native:web:WebApp                             functionsApp              create     
- +   ├─ azure-native:apimanagement:Api                      partnerApi                create     
- +   ├─ azure-native:apimanagement:ProductApi               partnerProductApi         create     
- +   └─ azure-native:web:WebApp                             partnerPortalApp          create     
-Diagnostics:
-  pulumi:pulumi:Stack (integrations-uat):
-    project: ... | location: AustraliaEast | stack: uat | env: uat | consumption: False | production: False | (preview)
-    error: Running program '/Users/.../bin/Debug/netcoreapp3.1/Infrastructure.dll' failed with an unhandled exception:
-    Grpc.Core.RpcException: Status(StatusCode="Unknown", Detail="invocation of azure-native:web:listWebAppHostKeys returned an error: request failed /subscriptions/.../resourceGroups/res-uat/providers/Microsoft.Web/sites/fn-uat/host/default/listkeys: autorest/azure: Service returned an error. Status=404 Code="ResourceNotFound" Message="The Resource 'Microsoft.Web/sites/fn-uat' under resource group 'res-uat' was not found. For more details please go to https://aka.ms/ARMResourceNotFoundFix"", DebugException="Grpc.Core.Internal.CoreErrorDetailException: {"created":"@1620789602.902369000","description":"Error received from peer ipv4:127.0.0.1:64203","file":"/tmpfs/src/github/grpc/workspace_csharp_ext_macos_x64/src/core/lib/surface/call.cc","file_line":1063,"grpc_message":"invocation of azure-native:web:listWebAppHostKeys returned an error: request failed /subscriptions/.../resourceGroups/res-uat/providers/Microsoft.Web/sites/fn-uat/host/default/listkeys: autorest/azure: Service returned an error. Status=404 Code="ResourceNotFound" Message="The Resource 'Microsoft.Web/sites/fn-uat' under resource group 'res-uat' was not found. For more details please go to https://aka.ms/ARMResourceNotFoundFix"","grpc_status":2}")
-       at Pulumi.GrpcMonitor.InvokeAsync(InvokeRequest request)
-       at Pulumi.Deployment.InvokeRawAsync(String token, InvokeArgs args, InvokeOptions options)
-       at Pulumi.Deployment.InvokeAsync[T](String token, InvokeArgs args, InvokeOptions options, Boolean convertResult)
-       at Pulumi.Output`1.ApplyHelperAsync[U](Task`1 dataTask, Func`2 func)
-       at Pulumi.Output`1.ApplyHelperAsync[U](Task`1 dataTask, Func`2 func)
-       at Pulumi.Serialization.Serializer.SerializeAsync(String ctx, Object prop, Boolean keepResources)
-       at Pulumi.Serialization.Serializer.SerializeAsync(String ctx, Object prop, Boolean keepResources)
-       at Pulumi.Deployment.SerializeFilteredPropertiesAsync(String label, IDictionary`2 args, Predicate`1 acceptKey, Boolean keepResources)
-       at Pulumi.Serialization.Serializer.SerializeAsync(String ctx, Object prop, Boolean keepResources)
-       at Pulumi.Deployment.SerializeFilteredPropertiesAsync(String label, IDictionary`2 args, Predicate`1 acceptKey, Boolean keepResources)
-       at Pulumi.Deployment.PrepareResourceAsync(String label, Resource res, Boolean custom, Boolean remote, ResourceArgs args, ResourceOptions options)
-       at Pulumi.Deployment.SerializeAllPropertiesAsync(String label, IDictionary`2 args, Boolean keepResources)
-       at Pulumi.Deployment.RegisterResourceOutputsAsync(Resource resource, Output`1 outputs)
-       at Pulumi.Deployment.RegisterResourceAsync(Resource resource, Boolean remote, Func`2 newDependency, ResourceArgs args, ResourceOptions options)
-       at Pulumi.Deployment.Runner.&lt;&gt;c__DisplayClass9_0.&lt;&lt;WhileRunningAsync&gt;g__HandleCompletion|0&gt;d.MoveNext()
-    --- End of stack trace from previous location where exception was thrown ---
-       at Pulumi.Output`1.GetValueAsync()
-       at Pulumi.Deployment.Logger.TryGetResourceUrnAsync(Resource resource)
-       at Pulumi.Output`1.ApplyHelperAsync[U](Task`1 dataTask, Func`2 func)
-       at Pulumi.Output`1.ApplyHelperAsync[U](Task`1 dataTask, Func`2 func)
-       at Pulumi.Output`1.&lt;TupleHelperAsync&gt;g__GetData|20_0[T1,T2,T3,T4,T5,T6,T7,T8,X](Input`1 input)
-       at Pulumi.Output`1.TupleHelperAsync[T1,T2,T3,T4,T5,T6,T7,T8](Input`1 item1, Input`1 item2, Input`1 item3, Input`1 item4, Input`1 item5, Input`1 item6, Input`1 item7, Input`1 item8)
-       at Pulumi.Output`1.ApplyHelperAsync[U](Task`1 dataTask, Func`2 func)
-       at Pulumi.Output`1.ApplyHelperAsync[U](Task`1 dataTask, Func`2 func)
-       at Pulumi.Output`1.Pulumi.IOutput.GetDataAsync()
-       at Pulumi.Serialization.Serializer.SerializeAsync(String ctx, Object prop, Boolean keepResources)
-       at Pulumi.Serialization.Serializer.SerializeAsync(String ctx, Object prop, Boolean keepResources)
-       at Pulumi.Serialization.Serializer.SerializeDictionaryAsync(String ctx, IDictionary dictionary, Boolean keepResources)
-       at Pulumi.Serialization.Serializer.SerializeInputArgsAsync(String ctx, InputArgs args, Boolean keepResources)
-       at Pulumi.Serialization.Serializer.SerializeAsync(String ctx, Object prop, Boolean keepResources)
-       at Pulumi.Serialization.Serializer.SerializeAsync(String ctx, Object prop, Boolean keepResources)
-       at Pulumi.Serialization.Serializer.SerializeAsync(String ctx, Object prop, Boolean keepResources)
-       at Pulumi.Deployment.SerializeFilteredPropertiesAsync(String label, IDictionary`2 args, Predicate`1 acceptKey, Boolean keepResources)
-       at Pulumi.Deployment.PrepareResourceAsync(String label, Resource res, Boolean custom, Boolean remote, ResourceArgs args, ResourceOptions options)
-       at Pulumi.Deployment.RegisterResourceAsync(Resource resource, Boolean remote, Func`2 newDependency, ResourceArgs args, ResourceOptions options)
-       at Pulumi.Deployment.ReadOrRegisterResourceAsync(Resource resource, Boolean remote, Func`2 newDependency, ResourceArgs args, ResourceOptions options)
-       at Pulumi.Deployment.CompleteResourceAsync(Resource resource, Boolean remote, Func`2 newDependency, ResourceArgs args, ResourceOptions options, ImmutableDictionary`2 completionSources)
-       at Pulumi.Output`1.GetValueAsync()
-       at Pulumi.Deployment.Logger.TryGetResourceUrnAsync(Resource resource)
-       at Pulumi.Output`1.ApplyHelperAsync[U](Task`1 dataTask, Func`2 func)
-       at Pulumi.Output`1.Pulumi.IOutput.GetDataAsync()
-       at Pulumi.Serialization.Serializer.SerializeAsync(String ctx, Object prop, Boolean keepResources)
-       at Pulumi.Serialization.Serializer.SerializeAsync(String ctx, Object prop, Boolean keepResources)
-       at Pulumi.Deployment.SerializeFilteredPropertiesAsync(String label, IDictionary`2 args, Predicate`1 acceptKey, Boolean keepResources)
-       at Pulumi.Deployment.PrepareResourceAsync(String label, Resource res, Boolean custom, Boolean remote, ResourceArgs args, ResourceOptions options)
-```
-## Affected feature
-pulumi up preview
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/34</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[Hackathon] Investigate options for publishing single-file binaries from .NET</x:t>
-  </x:si>
-  <x:si>
-    <x:t>As part of improving the authoring experience for multi-language component Pulumi Packages in pulumi/pulumi#6804, we should investigate if there is a good solution in .NET for generating a single-file binary with no dependencies (e.g. no requirement to install the .NET SDK). Potential candidates:
-- [.NET single file distribution](https://docs.microsoft.com/en-us/dotnet/core/deploying/single-file)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/35</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Set a NuGet package type in created NuGet packages</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Per a Loic Sharma on Twitter:
-&gt; Hi for Pulumi packages, y'all may want to consider using a custom NuGet package type. This would let you filter search results to just Pulumi packages, For example, if you create a package type "pulumi" you could then use that as a filter in search results: https://www.nuget.org/packages?packagetype=pulumi
-https://docs.microsoft.com/en-us/nuget/create-packages/set-package-type
-</x:t>
   </x:si>
   <x:si>
     <x:t>https://github.com/pulumi/pulumi-dotnet/issues/36</x:t>
@@ -4752,155 +3306,6 @@
 In current design Pulumi CLI and dotnet SDK exchange JSON messages over a file: EngineEvent, StdoutEngineEvent, DiagnosticEvent, and similar. This is a protocol that is not supported by an explicit schema tool like protobufs, so we need to remember to update the SDK when changes are made to these event objects. The idea here is to introduce some test that would serve as a reminder when they detect such changes.
 ## Affected feature
 Structured logging in dotnet.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/37</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Boilerplate repo for creating multi-lang component provider in .NET</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Depends on pulumi/pulumi-dotnet#46</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/42</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Import: program generation fails on '$default' property name</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Using the CLI import command for an IotHubResource gives...
-Still seems to get imported, but is everything okay?
-```
-error: internal error: Error: Invalid character
-  on anonymous.pp line 137:
- 138: $default ={
-This character is not used within the language.
-Error: Invalid expression
-  on anonymous.pp line 137:
- 138: $default ={
-Expected the start of an expression, but found an invalid expression token.
-```</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/43</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[sdk/dotnet] Use simpler types for relaxed enums</x:t>
-  </x:si>
-  <x:si>
-    <x:t>It seems like the (C#) typing can be simplified to something more understandable by the common developer.
-For instance, in AzureNextGen, `VaultArgs.Properties.AccessPolicies.Permissions` currently has the following definitions:
-```csharp
-public InputList&lt;Union&lt;string, CertificatePermissions&gt;&gt; Certificates;
-public InputList&lt;Union&lt;string, KeyPermissions&gt;&gt; Keys;
-public InputList&lt;Union&lt;string, SecretPermissions&gt;&gt; Secrets;
-public InputList&lt;Union&lt;string, StoragePermissions&gt;&gt; Storage;
-```
-And the Azure version has much simpler definitions:
-```csharp
-public InputList&lt;string&gt; CertificatePermissions;
-public InputList&lt;string&gt; KeyPermissions;
-public InputList&lt;string&gt; SecretPermissions;
-public InputList&lt;string&gt; StoragePermissions;
-```
-The move to use enum-like strings is a huge benefit, but the casual developer isn't going to understand what `Union&lt;string, KeyPermissions&gt;` is supposed to mean.
-Instead I recommend we simplify down to:
-```csharp
-public InputList&lt;CertificatePermissions&gt; Certificates;
-public InputList&lt;KeyPermissions&gt; Keys;
-public InputList&lt;SecretPermissions&gt; Secrets;
-public InputList&lt;StoragePermissions&gt; Storage;
-```
-This is doable by adding one line of code (for each type):
-```csharp
-public static implicit operator KeyPermissions(string value) =&gt; new KeyPermissions(value);
-```
-And makes things much clearer!
-UPDATE:
-The Azure SDK uses a public constructor instead. If we went that route, we would only need change the method constructor from `private` to `public`.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/44</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[codegen/dotnet] - Implement boolean enums</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/47</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[codegen/dotnet] Input/Output types don't mark deprecated properties as obsolete</x:t>
-  </x:si>
-  <x:si>
-    <x:t>For example:
-[Node.js](https://github.com/pulumi/pulumi-azure/blob/b71f7a61f0768215f8641b812b929fe20305c23d/sdk/nodejs/types/input.ts#L1366-L1369):
-```typescript
-        /**
-         * @deprecated This field has been deprecated in favour of `virtual_network_subnet_id` and will be removed in a future version of the provider
-         */
-        subnetId?: pulumi.Input&lt;string&gt;;
-```
-[.NET](https://github.com/pulumi/pulumi-azure/blob/8250f3f0fdab84a9e17c5307a16fe53922cebe74/sdk/dotnet/AppService/Inputs/AppServiceSiteConfigIpRestrictionArgs.cs#L39-L40):
-```c#
-        [Input("subnetId")]
-        public Input&lt;string&gt;? SubnetId { get; set; }
-```</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/48</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C# project with launchSettings.json causes diagnostic messages</x:t>
-  </x:si>
-  <x:si>
-    <x:t>While experimenting with Visual Studio [`launchSettings.json`](https://docs.microsoft.com/en-us/visualstudio/containers/container-launch-settings) in a Pulumi C# project:
-```json
-{
-  "profiles": {
-    "Pulumi": {
-      "commandName": "Executable",
-      "executablePath": "pulumi",
-      "commandLineArgs": "preview --non-interactive --stack=org/alpha",
-      "environmentVariables": {
-        "PULUMI_DEBUG": "true"
-      }
-    }
-  }
-}
-```
-... I started getting the following diagnostic messages during `pulumi preview`:
-```
-Diagnostics:
-  pulumi:pulumi:Stack (stack-alpha):
-    The launch profile "(Default)" could not be applied.
-    A usable launch profile could not be located.
-```
-... and if I delete the `launchSettings.json` file then the diagnostic messages disappear.
-It looks like this is due to the way `pulumi` shells out to [`dotnet run`](https://docs.microsoft.com/en-us/dotnet/core/tools/dotnet-run) and, since this file is irrelevant in that case, I think this would be fixed by `pulumi` also passing the `--no-launch-profile` option to `dotnet run`.
-&gt; Doesn't try to use launchSettings.json to configure the application.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/49</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Better tooltip text for VS Code?</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">The tooltip text in VS Code seems to have some formatting issues.
-### Example 1
-```
-public InputList&lt;string&gt; SubnetCidrBlock { get; set; } = null!;
-```
-shows this in the tooltip:
-![image](https://user-images.githubusercontent.com/293763/87639567-4893f080-c6fa-11ea-8cf9-f60b67d9f5b2.png)
-### Example 2 
-```
-public Input&lt;string&gt; SubnetCidrBlock { get; set; } = null!;
-``` 
-shows this in the tooltip:
-![image](https://user-images.githubusercontent.com/293763/87639863-b93b0d00-c6fa-11ea-8692-1797b3552809.png)
-</x:t>
   </x:si>
   <x:si>
     <x:t>https://github.com/pulumi/pulumi-dotnet/issues/50</x:t>
@@ -4943,331 +3348,6 @@
         /// &lt;/example&gt;
 ```
 Consider applying this format to the generated C# code to improve Intellisense and DocFX docs.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/51</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Inconsistent behaviour accessing AppService Parameters</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> I have created an Azure App Service using C# and specified the following (abbreviated) args
-`var webApp = new AppService(name, new AppServiceArgs
-{
-    ClientAffinityEnabled = false,
-    HttpsOnly = true,
-}`
-I can access the value for ClientAffinityEnabled like this
-`var temp = webApp.ClientAffinityEnabled;`
-but that doesn't work for the value of HttpsOnly which I have to access using Apply like
-`var temp = webApp.HttpsOnly.Apply(v =&gt; v!.Value);`
-Mikhail suggested in Slack that this was due to an issue with the "duality of nullable types in C# (value vs reference)" and asked me to raise this issue for it ([original question in slack](https://pulumi-community.slack.com/archives/CQ2QFLNFL/p1589623937100600))</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/52</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Proposal: strongly-typed API to specify secret outputs (dotnet)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Specifying that some resources' outputs should be secret currently works like this:
-```csharp
-var secret = new RandomPassword("my-random-password",
-    new RandomPasswordArgs
-    {
-        Length = 30,
-        Special = true,
-    },
-    new CustomResourceOptions
-    {
-        AdditionalSecretOutputs = new List&lt;string&gt;
-        {
-            "result" // stringly-typed API, no compiler feedback for typos, etc.
-        }
-    });
-```
-I propose an alternative approach so that end-users can specify secrets in a strongly-typed way to prevent a mistyped string from potentially leaking secrets at runtime and/or failing at runtime:
-```csharp
-var secret = new RandomPassword("my-random-password",
-    new RandomPasswordArgs
-    {
-        Length = 30,
-        Special = true,
-    },
-    new CustomResourceOptions&lt;RandomPassword&gt;() // specify generic for strong typing
-        .AddSecretOutput(x =&gt; x.Result) // specify output via expression; typos yield compiler errors
-    );
-```</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/53</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Pulumi does not respect Output properties defined in base classes</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">If you use your own base class and define an Output property like this:
-```csharp
-// Custom Base class BaseStack: Stack
-[Output] public Output&lt;string&gt; OutputA { get; set; } = Output.Create("a");
-```
-`pulumi up` does not recognize `OutputA` as a change.
-If you put the property on the beginning of the hierarchie (MyStack --&gt; BaseStack --&gt; Stack), everything works fine.
-```csharp
-// class MyStack: BaseStack
-[Output] public Output&lt;string&gt; OutputA { get; set; } = Output.Create("a");
-```
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/54</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Better support for defining Pulumi conventions in .NET</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">I have 3 requirements, which I would like to implement as a convention in Pulumi.
-- By default all AppServices must be HttpsOnly
-- All resources must have a speficied set of tags
-- All resources belong into one resource group
-```csharp
-private static ResourceTransformationResult? Transform(ResourceTransformationArgs args)
-{
-    if (args.Args is AppServiceArgs serviceArgs)
-    {
-        serviceArgs.HttpsOnly = true;
-    }
-    var tagsProperty = args.Args.GetType().GetProperty("Tags");
-    if (tagsProperty != null) tagsProperty.SetValue(args.Args, GetTags());
-    var resourceGroupNameProperty = args.Args.GetType().GetProperty("ResourceGroupName");
-    if (resourceGroupNameProperty != null) resourceGroupNameProperty.SetValue(args.Args, (Input&lt;string&gt;)ResourceGroupName);
-    return new ResourceTransformationResult(args.Args, args.Options);
-}
-```
-As you can there is no other way than using reflection to get the `Tags` and `ResourceGroupName` property. 
-It would be nice to have a better object model for resources (e.g. Marker Interfaces). 
-Alternatively a specialised DSL could also be ok.
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/55</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Support for Solution file in .NET Core</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I have one csproj file within one Visual Studio solution. 
-When I run `pulumi up` I get the following error:
-&gt;  MSBUILD : error MSB1050: Specify which project or solution file to use because the folder "." contains more than one project or solution file.
-Please make it possible to explicitly pass in the correct csproj file via pulumi console or pulumi stack configuration or determine the csproj file automatically and pass it to msbuild.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/56</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Do not require public setters on .NET Stacks</x:t>
-  </x:si>
-  <x:si>
-    <x:t>A small but annoying implementation detail. The following code:
-```cs
-class ValidStack : Stack
- {
-    [Output]
-    public Output&lt;string&gt; Foo { get; }
-    public ValidStack()
-    {
-       this.Foo = Output.Create("bar");
-    }
-}
-```
-is perfectly valid C# code but will fail at runtime because there's no public setter on `Foo`. That's a reasonable requirement for Custom Resources but not for Stacks. A stack is responsible for instantiating its own outputs and they are [validated separately](https://github.com/pulumi/pulumi/blob/master/sdk/dotnet/Pulumi/Stack.cs#L89).
-IDEs may give a refactoring suggestion to remove unused setters on stack classes, which unexpectedly break the program. Because this applies to almost all .NET stacks ever, I think it's worth relaxing the check.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/57</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Create method/extensions to allow math on Output and Input Variables (.NET)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>When I have input variables such or even output variables from a lookup that are int types I cannot add these variables together.
-```c#
-var int1 = args.VmTemplate.Apply(x =&gt; x.Disks[0].Size ) + args.SrvExtendSize
-// or even
-var int2 = args.VmTemplate.Apply(x =&gt; x.Disks[0].Size ) + args.SrvExtendSize.ToOutput()
-```
-The only way to successfully get this to work was to use the Tuple method which is a lot just to add two numbers.
-```c#
-var int = Output.Tuple(args.VmTemplate, args.SrvExtendSize).Apply(t =&gt; {
-    var (template, extendedSize) = t;
-    return template.Disks[0].Size + extendedSize;
-});
-```
-I am proposing that extension methods be created to allow adding/subtracting/diving/multiplying, etc. output and input variables or even overloading the operators but that wont work with all languages. This would make it much easier.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/58</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Serialization failure exporting an `[OutputType]` class as a stack export in .NET</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I get this:
-```
- System.InvalidOperationException: Pulumi.Kubernetes.Types.Outputs.Rbac.V1.Subject is not a supported argument type.
-        monitor.registerResourceOutputs(...).subjects.id[0]
-       at Pulumi.Serialization.Serializer.SerializeAsync(String ctx, Object prop)
-       at Pulumi.Serialization.Serializer.SerializeListAsync(String ctx, IList list)
-```
-When trying to return to add the last line (`subjects`) below:
-```cs
-             return new Dictionary&lt;string, object&gt;{
-                { "namespacePhase", ns.Status.Apply(status =&gt; status.Phase) },
-                { "revisionData", revision.Data },
-                { "subjects", binding.Subjects },
-            };
-```
-The type of that property is:
-```cs
-Output&lt;System.Collections.Immutable.ImmutableArray&lt;Pulumi.Kubernetes.Types.Outputs.Rbac.V1.Subject&gt;&gt; RoleBinding.Subjects
-```
-It appears that the serialization we do for `registerResourceOutputs` and/or stack exports is not correctly supporting `OutputType` classes.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/59</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Idiomatic F# API</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Pulumi .NET SDK supports F# as one of the languages to author infrastructure programs. It works quite fine, but there are several complications which make F# programs harder to write.
-A typical Pulumi program consists of a number of value assignments, each calling a constructor of a resource type with proper arguments. The resource is defined by virtue of calling its constructor: the value doesn't need to be returned or passed to anywhere.
-Let's look at two existing examples:
-**A. Azure resources ([full code](https://github.com/pulumi/examples/blob/master/azure-fs-appservice/Program.fs)):**
-``` fsharp
-let resourceGroup = ResourceGroup "appservice-rg"
-let storageAccount =
-    Account("sa",
-        AccountArgs
-           (ResourceGroupName = io resourceGroup.Name,
-            AccountReplicationType = input "LRS",
-            AccountTier = input "Standard"))
-let sku = PlanSkuArgs(Tier = input "Basic", Size = input "B1")
-let appServicePlan = 
-    Plan("asp", 
-        PlanArgs
-           (ResourceGroupName = io resourceGroup.Name,
-            Kind = input "App",
-            Sku = input sku))
-```
-**B. Kubernetes deployment ([full code](https://github.com/pulumi/templates/blob/master/kubernetes-fsharp/Program.fs)):**
-``` fsharp
-let deployment = 
-    Pulumi.Kubernetes.Apps.V1.Deployment("nginx",
-      DeploymentArgs
-        (Spec = input (DeploymentSpecArgs
-          (Selector = input (LabelSelectorArgs(MatchLabels = appLabels)),
-           Replicas = input 1,
-           Template = input (
-             PodTemplateSpecArgs
-              (Metadata = input (ObjectMetaArgs(Labels = appLabels)),
-               Spec = input (
-                  PodSpecArgs
-                    (Containers = 
-                      inputList [
-                        input (
-                          ContainerArgs
-                            (Name = input "nginx",
-                             Image = input "nginx",
-                             Ports = 
-                              inputList [
-                                input (
-                                 ContainerPortArgs
-                                   (ContainerPortValue = input 80))]))]))))))))
-```
-Here are some challenges:
-### 1. Inputs and outputs.
-Resources may contain output values: e.g. `resourceGroup.Name` in the first snippet. Its value might not be known at the time when this property is used, so a special type `Output&lt;T&gt;` is used to define the outputs. It's somewhat similar to `Task&lt;T&gt;`.
-Each resource's constructor accepts a property bag where each property typically has type `Input&lt;T&gt;` or a type derived from it. An input can be a plain value (`1`, `"nginx") or point to an output value of another resource. This allows chaining the resources and creating dependencies between them.
-While C# has implicit conversions between plain values, outputs, and inputs, F# type system is strict and requires conversions. Helper functions `input`, `io`, `inputList`, etc. were created to simplify the conversions, but they still clutter the code, and might be tricky to get right at times.
-### 2. Indentation.
-F# is white space significant, so the indentations must be right. The kubernetes example above shows that some resource args may use subtypes and sub-sub-types etc, so indentation gets quite heavy. It's also very strict, and compiler messages are not very helpful in getting it right.
-Going one level deeper requires a `(` or `[`, so the final statement ends with something like `))]))]))))))))`.
-### 3. Side effects.
-Resources are defined by calling constructors. Effectively, Pulumi SDK is based on side effects of calling those constructors as opposed to pure functions returning results. This goes against F# philosophy and puts an obstacle against many useful functional techniques.
----
-For inspiration, a comparable kubernetes example in TypeScript looks much more concise:
-``` ts
-const deployment = new k8s.apps.v1.Deployment("nginx", {
-    spec: {
-        selector: { matchLabels: appLabels },
-        replicas: 1,
-        template: {
-            metadata: { labels: appLabels },
-            spec: { containers: [{ name: "nginx", image: "nginx" }] }
-        }
-    }
-});
-```
-The goal is to bring readability and write-ability of F# programs close to this level.
----
-Good places to give a try to a Pulumi program in F#:
-- [Getting Started with Kubernetes](https://www.pulumi.com/docs/get-started/kubernetes/install-pulumi/) - use `kubernetes-fsharp` template when asked ([link to the template](https://github.com/pulumi/templates/tree/master/kubernetes-fsharp)]
-- [Azure AppService example](https://github.com/pulumi/examples/tree/master/azure-fs-appservice)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/60</x:t>
-  </x:si>
-  <x:si>
-    <x:t>.NET SDK: allow arbitrary objects to be exported from a stack</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">We could convert them to POCOs and export those (like we do with js/ts/python).  </x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/61</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Callback serialization for .NET</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Investigate callback serialization for .NET to support things like callback-based serverless functions</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/62</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Investigate 'lifting' on .NET outputs</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Given some
-``` csharp
-class A
-{ 
-    public int Value { get; } 
-}
-Output&lt;A&gt; output = ...; 
-```
-to get to the value we need to do `output.Apply(o =&gt; o.Value)` while in Node.js we could do `output.value` in a similar situation.
-We should investigate whether a similar experience in possible in C#.
-One avenue is to generate extension methods for each property:
-``` csharp
-static class Extensions
-{
-    public Output&lt;int&gt; Value(this Output&lt;A&gt; a) =&gt; a.Apply(o =&gt; o.Value);
-}
-var value = output.Value();
-```
-Related: https://github.com/pulumi/pulumi/pull/3481#discussion_r344507398</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://github.com/pulumi/pulumi-dotnet/issues/63</x:t>
-  </x:si>
-  <x:si>
-    <x:t>.NET Dynamic Providers</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Pulumi .NET SDK currently does not support [Dynamic Resource Providers](https://www.pulumi.com/docs/concepts/resources/dynamic-providers/). </x:t>
   </x:si>
   <x:si>
     <x:t>https://github.com/proti-iac/proti/issues/18</x:t>
@@ -5668,11 +3748,11 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="39.585625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="101.335625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="15.960625" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="9.210625" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="15.960625" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="45.567768" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="109.567768" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="16.282054" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="9.567768" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="16.567768" style="0" customWidth="1"/>
     <x:col min="6" max="6" width="255" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
@@ -7950,17 +6030,17 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:F96"/>
+  <x:dimension ref="A1:F34"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="43.460625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="90.585625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="15.960625" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="9.210625" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="15.960625" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="50.282054" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="92.567768" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="16.282054" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="9.567768" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="16.567768" style="0" customWidth="1"/>
     <x:col min="6" max="6" width="255" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
@@ -7992,7 +6072,7 @@
         <x:v>342</x:v>
       </x:c>
       <x:c r="C2" s="2">
-        <x:v>45763.4639699074</x:v>
+        <x:v>45723.9116435185</x:v>
       </x:c>
       <x:c r="D2" s="0">
         <x:v>0</x:v>
@@ -8012,7 +6092,7 @@
         <x:v>345</x:v>
       </x:c>
       <x:c r="C3" s="2">
-        <x:v>45755.8736689815</x:v>
+        <x:v>45708.4314583333</x:v>
       </x:c>
       <x:c r="D3" s="0">
         <x:v>0</x:v>
@@ -8032,7 +6112,7 @@
         <x:v>348</x:v>
       </x:c>
       <x:c r="C4" s="2">
-        <x:v>45751.8293981481</x:v>
+        <x:v>45708.1901736111</x:v>
       </x:c>
       <x:c r="D4" s="0">
         <x:v>0</x:v>
@@ -8040,7 +6120,7 @@
       <x:c r="E4" s="0">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="F4" s="0" t="s">
+      <x:c r="F4" s="3" t="s">
         <x:v>349</x:v>
       </x:c>
     </x:row>
@@ -8052,7 +6132,7 @@
         <x:v>351</x:v>
       </x:c>
       <x:c r="C5" s="2">
-        <x:v>45723.9116435185</x:v>
+        <x:v>45708.1896180556</x:v>
       </x:c>
       <x:c r="D5" s="0">
         <x:v>0</x:v>
@@ -8072,7 +6152,7 @@
         <x:v>354</x:v>
       </x:c>
       <x:c r="C6" s="2">
-        <x:v>45713.447974537</x:v>
+        <x:v>45708.1891087963</x:v>
       </x:c>
       <x:c r="D6" s="0">
         <x:v>0</x:v>
@@ -8092,7 +6172,7 @@
         <x:v>357</x:v>
       </x:c>
       <x:c r="C7" s="2">
-        <x:v>45708.4314583333</x:v>
+        <x:v>45707.6379861111</x:v>
       </x:c>
       <x:c r="D7" s="0">
         <x:v>0</x:v>
@@ -8112,7 +6192,7 @@
         <x:v>360</x:v>
       </x:c>
       <x:c r="C8" s="2">
-        <x:v>45708.1901736111</x:v>
+        <x:v>45707.4038541667</x:v>
       </x:c>
       <x:c r="D8" s="0">
         <x:v>0</x:v>
@@ -8132,7 +6212,7 @@
         <x:v>363</x:v>
       </x:c>
       <x:c r="C9" s="2">
-        <x:v>45708.1896180556</x:v>
+        <x:v>45630.6213541667</x:v>
       </x:c>
       <x:c r="D9" s="0">
         <x:v>0</x:v>
@@ -8152,7 +6232,7 @@
         <x:v>366</x:v>
       </x:c>
       <x:c r="C10" s="2">
-        <x:v>45708.1891087963</x:v>
+        <x:v>45617.6777430556</x:v>
       </x:c>
       <x:c r="D10" s="0">
         <x:v>0</x:v>
@@ -8172,7 +6252,7 @@
         <x:v>369</x:v>
       </x:c>
       <x:c r="C11" s="2">
-        <x:v>45707.6379861111</x:v>
+        <x:v>45612.0007175926</x:v>
       </x:c>
       <x:c r="D11" s="0">
         <x:v>0</x:v>
@@ -8192,13 +6272,13 @@
         <x:v>372</x:v>
       </x:c>
       <x:c r="C12" s="2">
-        <x:v>45707.4038541667</x:v>
+        <x:v>45610.2021643519</x:v>
       </x:c>
       <x:c r="D12" s="0">
-        <x:v>0</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="E12" s="0">
-        <x:v>0</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="F12" s="3" t="s">
         <x:v>373</x:v>
@@ -8212,7 +6292,7 @@
         <x:v>375</x:v>
       </x:c>
       <x:c r="C13" s="2">
-        <x:v>45706.3469791667</x:v>
+        <x:v>45608.6264930556</x:v>
       </x:c>
       <x:c r="D13" s="0">
         <x:v>0</x:v>
@@ -8220,7 +6300,7 @@
       <x:c r="E13" s="0">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="F13" s="3" t="s">
+      <x:c r="F13" s="0" t="s">
         <x:v>376</x:v>
       </x:c>
     </x:row>
@@ -8232,24 +6312,27 @@
         <x:v>378</x:v>
       </x:c>
       <x:c r="C14" s="2">
-        <x:v>45685.7564236111</x:v>
+        <x:v>45582.5868518519</x:v>
       </x:c>
       <x:c r="D14" s="0">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="E14" s="0">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F14" s="3" t="s">
+        <x:v>379</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:6">
       <x:c r="A15" s="0" t="s">
-        <x:v>379</x:v>
+        <x:v>380</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>380</x:v>
+        <x:v>381</x:v>
       </x:c>
       <x:c r="C15" s="2">
-        <x:v>45671.1957986111</x:v>
+        <x:v>45544.4907638889</x:v>
       </x:c>
       <x:c r="D15" s="0">
         <x:v>0</x:v>
@@ -8258,18 +6341,18 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="F15" s="3" t="s">
-        <x:v>381</x:v>
+        <x:v>382</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:6">
       <x:c r="A16" s="0" t="s">
-        <x:v>382</x:v>
+        <x:v>383</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>383</x:v>
+        <x:v>384</x:v>
       </x:c>
       <x:c r="C16" s="2">
-        <x:v>45630.6213541667</x:v>
+        <x:v>45464.7875578704</x:v>
       </x:c>
       <x:c r="D16" s="0">
         <x:v>0</x:v>
@@ -8278,18 +6361,18 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="F16" s="3" t="s">
-        <x:v>384</x:v>
+        <x:v>385</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:6">
       <x:c r="A17" s="0" t="s">
-        <x:v>385</x:v>
+        <x:v>386</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>386</x:v>
+        <x:v>387</x:v>
       </x:c>
       <x:c r="C17" s="2">
-        <x:v>45618.6899768518</x:v>
+        <x:v>45237.4165046296</x:v>
       </x:c>
       <x:c r="D17" s="0">
         <x:v>1</x:v>
@@ -8298,18 +6381,18 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="F17" s="3" t="s">
-        <x:v>387</x:v>
+        <x:v>388</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:6">
       <x:c r="A18" s="0" t="s">
-        <x:v>388</x:v>
+        <x:v>389</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>389</x:v>
+        <x:v>390</x:v>
       </x:c>
       <x:c r="C18" s="2">
-        <x:v>45617.6777430556</x:v>
+        <x:v>45169.3445949074</x:v>
       </x:c>
       <x:c r="D18" s="0">
         <x:v>0</x:v>
@@ -8317,19 +6400,19 @@
       <x:c r="E18" s="0">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="F18" s="3" t="s">
-        <x:v>390</x:v>
+      <x:c r="F18" s="0" t="s">
+        <x:v>391</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:6">
       <x:c r="A19" s="0" t="s">
-        <x:v>391</x:v>
+        <x:v>392</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>392</x:v>
+        <x:v>393</x:v>
       </x:c>
       <x:c r="C19" s="2">
-        <x:v>45617.6629861111</x:v>
+        <x:v>45162.5534259259</x:v>
       </x:c>
       <x:c r="D19" s="0">
         <x:v>0</x:v>
@@ -8338,18 +6421,18 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="F19" s="3" t="s">
-        <x:v>393</x:v>
+        <x:v>394</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:6">
       <x:c r="A20" s="0" t="s">
-        <x:v>394</x:v>
+        <x:v>395</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>395</x:v>
+        <x:v>396</x:v>
       </x:c>
       <x:c r="C20" s="2">
-        <x:v>45617.2368287037</x:v>
+        <x:v>45131.3296990741</x:v>
       </x:c>
       <x:c r="D20" s="0">
         <x:v>0</x:v>
@@ -8358,18 +6441,18 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="F20" s="3" t="s">
-        <x:v>396</x:v>
+        <x:v>397</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:6">
       <x:c r="A21" s="0" t="s">
-        <x:v>397</x:v>
+        <x:v>398</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>398</x:v>
+        <x:v>399</x:v>
       </x:c>
       <x:c r="C21" s="2">
-        <x:v>45612.0007175926</x:v>
+        <x:v>45110.506400463</x:v>
       </x:c>
       <x:c r="D21" s="0">
         <x:v>0</x:v>
@@ -8378,178 +6461,178 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="F21" s="3" t="s">
-        <x:v>399</x:v>
+        <x:v>400</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:6">
       <x:c r="A22" s="0" t="s">
-        <x:v>400</x:v>
+        <x:v>401</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>401</x:v>
+        <x:v>402</x:v>
       </x:c>
       <x:c r="C22" s="2">
-        <x:v>45610.2021643519</x:v>
+        <x:v>45065.9196180556</x:v>
       </x:c>
       <x:c r="D22" s="0">
-        <x:v>3</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="E22" s="0">
-        <x:v>3</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="F22" s="3" t="s">
-        <x:v>402</x:v>
+        <x:v>403</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:6">
       <x:c r="A23" s="0" t="s">
-        <x:v>403</x:v>
+        <x:v>404</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>404</x:v>
+        <x:v>405</x:v>
       </x:c>
       <x:c r="C23" s="2">
-        <x:v>45608.6264930556</x:v>
+        <x:v>45043.3846064815</x:v>
       </x:c>
       <x:c r="D23" s="0">
-        <x:v>0</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="E23" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F23" s="0" t="s">
-        <x:v>405</x:v>
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F23" s="3" t="s">
+        <x:v>406</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:6">
       <x:c r="A24" s="0" t="s">
-        <x:v>406</x:v>
+        <x:v>407</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>407</x:v>
+        <x:v>408</x:v>
       </x:c>
       <x:c r="C24" s="2">
-        <x:v>45607.6856481481</x:v>
+        <x:v>45023.8305439815</x:v>
       </x:c>
       <x:c r="D24" s="0">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="E24" s="0">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="F24" s="3" t="s">
-        <x:v>408</x:v>
+        <x:v>409</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:6">
       <x:c r="A25" s="0" t="s">
-        <x:v>409</x:v>
+        <x:v>410</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>410</x:v>
+        <x:v>411</x:v>
       </x:c>
       <x:c r="C25" s="2">
-        <x:v>45607.1505555556</x:v>
+        <x:v>44960.6602430556</x:v>
       </x:c>
       <x:c r="D25" s="0">
-        <x:v>4</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="E25" s="0">
-        <x:v>4</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="F25" s="3" t="s">
-        <x:v>411</x:v>
+        <x:v>412</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:6">
       <x:c r="A26" s="0" t="s">
-        <x:v>412</x:v>
+        <x:v>413</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>413</x:v>
+        <x:v>414</x:v>
       </x:c>
       <x:c r="C26" s="2">
-        <x:v>45595.476724537</x:v>
+        <x:v>44865.3693634259</x:v>
       </x:c>
       <x:c r="D26" s="0">
-        <x:v>1</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="E26" s="0">
-        <x:v>1</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="F26" s="3" t="s">
-        <x:v>414</x:v>
+        <x:v>415</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:6">
       <x:c r="A27" s="0" t="s">
-        <x:v>415</x:v>
+        <x:v>416</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>416</x:v>
+        <x:v>417</x:v>
       </x:c>
       <x:c r="C27" s="2">
-        <x:v>45590.6012962963</x:v>
+        <x:v>44818.6455555556</x:v>
       </x:c>
       <x:c r="D27" s="0">
-        <x:v>3</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="E27" s="0">
-        <x:v>3</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="F27" s="3" t="s">
-        <x:v>417</x:v>
+        <x:v>418</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:6">
       <x:c r="A28" s="0" t="s">
-        <x:v>418</x:v>
+        <x:v>419</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>419</x:v>
+        <x:v>420</x:v>
       </x:c>
       <x:c r="C28" s="2">
-        <x:v>45582.5868518519</x:v>
+        <x:v>44787.841712963</x:v>
       </x:c>
       <x:c r="D28" s="0">
-        <x:v>1</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="E28" s="0">
-        <x:v>1</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="F28" s="3" t="s">
-        <x:v>420</x:v>
+        <x:v>421</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:6">
       <x:c r="A29" s="0" t="s">
-        <x:v>421</x:v>
+        <x:v>422</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>422</x:v>
+        <x:v>423</x:v>
       </x:c>
       <x:c r="C29" s="2">
-        <x:v>45544.4907638889</x:v>
+        <x:v>44602.6183680556</x:v>
       </x:c>
       <x:c r="D29" s="0">
-        <x:v>0</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="E29" s="0">
-        <x:v>0</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="F29" s="3" t="s">
-        <x:v>423</x:v>
+        <x:v>424</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:6">
       <x:c r="A30" s="0" t="s">
-        <x:v>424</x:v>
+        <x:v>425</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>425</x:v>
+        <x:v>426</x:v>
       </x:c>
       <x:c r="C30" s="2">
-        <x:v>45524.5265740741</x:v>
+        <x:v>44557.8673263889</x:v>
       </x:c>
       <x:c r="D30" s="0">
         <x:v>0</x:v>
@@ -8558,18 +6641,18 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="F30" s="3" t="s">
-        <x:v>426</x:v>
+        <x:v>427</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:6">
       <x:c r="A31" s="0" t="s">
-        <x:v>427</x:v>
+        <x:v>428</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>428</x:v>
+        <x:v>429</x:v>
       </x:c>
       <x:c r="C31" s="2">
-        <x:v>45464.7875578704</x:v>
+        <x:v>44455.7410416667</x:v>
       </x:c>
       <x:c r="D31" s="0">
         <x:v>0</x:v>
@@ -8578,18 +6661,18 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="F31" s="3" t="s">
-        <x:v>429</x:v>
+        <x:v>430</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:6">
       <x:c r="A32" s="0" t="s">
-        <x:v>430</x:v>
+        <x:v>431</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>431</x:v>
+        <x:v>432</x:v>
       </x:c>
       <x:c r="C32" s="2">
-        <x:v>45369.4829050926</x:v>
+        <x:v>44385.8234722222</x:v>
       </x:c>
       <x:c r="D32" s="0">
         <x:v>0</x:v>
@@ -8598,18 +6681,18 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="F32" s="3" t="s">
-        <x:v>432</x:v>
+        <x:v>433</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:6">
       <x:c r="A33" s="0" t="s">
-        <x:v>433</x:v>
+        <x:v>434</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>434</x:v>
+        <x:v>435</x:v>
       </x:c>
       <x:c r="C33" s="2">
-        <x:v>45324.7824768519</x:v>
+        <x:v>44285.6562962963</x:v>
       </x:c>
       <x:c r="D33" s="0">
         <x:v>0</x:v>
@@ -8618,1261 +6701,27 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="F33" s="3" t="s">
-        <x:v>435</x:v>
+        <x:v>436</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:6">
       <x:c r="A34" s="0" t="s">
-        <x:v>436</x:v>
+        <x:v>437</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>437</x:v>
+        <x:v>438</x:v>
       </x:c>
       <x:c r="C34" s="2">
-        <x:v>45245.4743402778</x:v>
+        <x:v>44011.4896296296</x:v>
       </x:c>
       <x:c r="D34" s="0">
-        <x:v>3</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="E34" s="0">
-        <x:v>3</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="F34" s="3" t="s">
-        <x:v>438</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="35" spans="1:6">
-      <x:c r="A35" s="0" t="s">
         <x:v>439</x:v>
-      </x:c>
-      <x:c r="B35" s="0" t="s">
-        <x:v>440</x:v>
-      </x:c>
-      <x:c r="C35" s="2">
-        <x:v>45237.4165046296</x:v>
-      </x:c>
-      <x:c r="D35" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="E35" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F35" s="3" t="s">
-        <x:v>441</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="36" spans="1:6">
-      <x:c r="A36" s="0" t="s">
-        <x:v>442</x:v>
-      </x:c>
-      <x:c r="B36" s="0" t="s">
-        <x:v>443</x:v>
-      </x:c>
-      <x:c r="C36" s="2">
-        <x:v>45231.9502893519</x:v>
-      </x:c>
-      <x:c r="D36" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="E36" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F36" s="3" t="s">
-        <x:v>444</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="37" spans="1:6">
-      <x:c r="A37" s="0" t="s">
-        <x:v>445</x:v>
-      </x:c>
-      <x:c r="B37" s="0" t="s">
-        <x:v>446</x:v>
-      </x:c>
-      <x:c r="C37" s="2">
-        <x:v>45174.2994444444</x:v>
-      </x:c>
-      <x:c r="D37" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E37" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F37" s="3" t="s">
-        <x:v>447</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="38" spans="1:6">
-      <x:c r="A38" s="0" t="s">
-        <x:v>448</x:v>
-      </x:c>
-      <x:c r="B38" s="0" t="s">
-        <x:v>449</x:v>
-      </x:c>
-      <x:c r="C38" s="2">
-        <x:v>45169.3445949074</x:v>
-      </x:c>
-      <x:c r="D38" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E38" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F38" s="0" t="s">
-        <x:v>450</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="39" spans="1:6">
-      <x:c r="A39" s="0" t="s">
-        <x:v>451</x:v>
-      </x:c>
-      <x:c r="B39" s="0" t="s">
-        <x:v>452</x:v>
-      </x:c>
-      <x:c r="C39" s="2">
-        <x:v>45162.5534259259</x:v>
-      </x:c>
-      <x:c r="D39" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E39" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F39" s="3" t="s">
-        <x:v>453</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="40" spans="1:6">
-      <x:c r="A40" s="0" t="s">
-        <x:v>454</x:v>
-      </x:c>
-      <x:c r="B40" s="0" t="s">
-        <x:v>455</x:v>
-      </x:c>
-      <x:c r="C40" s="2">
-        <x:v>45156.8403125</x:v>
-      </x:c>
-      <x:c r="D40" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E40" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F40" s="3" t="s">
-        <x:v>456</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="41" spans="1:6">
-      <x:c r="A41" s="0" t="s">
-        <x:v>457</x:v>
-      </x:c>
-      <x:c r="B41" s="0" t="s">
-        <x:v>458</x:v>
-      </x:c>
-      <x:c r="C41" s="2">
-        <x:v>45131.3296990741</x:v>
-      </x:c>
-      <x:c r="D41" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E41" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F41" s="3" t="s">
-        <x:v>459</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="42" spans="1:6">
-      <x:c r="A42" s="0" t="s">
-        <x:v>460</x:v>
-      </x:c>
-      <x:c r="B42" s="0" t="s">
-        <x:v>461</x:v>
-      </x:c>
-      <x:c r="C42" s="2">
-        <x:v>45110.506400463</x:v>
-      </x:c>
-      <x:c r="D42" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E42" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F42" s="3" t="s">
-        <x:v>462</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="43" spans="1:6">
-      <x:c r="A43" s="0" t="s">
-        <x:v>463</x:v>
-      </x:c>
-      <x:c r="B43" s="0" t="s">
-        <x:v>464</x:v>
-      </x:c>
-      <x:c r="C43" s="2">
-        <x:v>45107.5944675926</x:v>
-      </x:c>
-      <x:c r="D43" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="E43" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F43" s="3" t="s">
-        <x:v>465</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="44" spans="1:6">
-      <x:c r="A44" s="0" t="s">
-        <x:v>466</x:v>
-      </x:c>
-      <x:c r="B44" s="0" t="s">
-        <x:v>467</x:v>
-      </x:c>
-      <x:c r="C44" s="2">
-        <x:v>45065.9196180556</x:v>
-      </x:c>
-      <x:c r="D44" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E44" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F44" s="3" t="s">
-        <x:v>468</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="45" spans="1:6">
-      <x:c r="A45" s="0" t="s">
-        <x:v>469</x:v>
-      </x:c>
-      <x:c r="B45" s="0" t="s">
-        <x:v>470</x:v>
-      </x:c>
-      <x:c r="C45" s="2">
-        <x:v>45043.3846064815</x:v>
-      </x:c>
-      <x:c r="D45" s="0">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="E45" s="0">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="F45" s="3" t="s">
-        <x:v>471</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="46" spans="1:6">
-      <x:c r="A46" s="0" t="s">
-        <x:v>472</x:v>
-      </x:c>
-      <x:c r="B46" s="0" t="s">
-        <x:v>473</x:v>
-      </x:c>
-      <x:c r="C46" s="2">
-        <x:v>45040.722337963</x:v>
-      </x:c>
-      <x:c r="D46" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E46" s="0">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="47" spans="1:6">
-      <x:c r="A47" s="0" t="s">
-        <x:v>474</x:v>
-      </x:c>
-      <x:c r="B47" s="0" t="s">
-        <x:v>475</x:v>
-      </x:c>
-      <x:c r="C47" s="2">
-        <x:v>45023.8305439815</x:v>
-      </x:c>
-      <x:c r="D47" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="E47" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F47" s="3" t="s">
-        <x:v>476</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="48" spans="1:6">
-      <x:c r="A48" s="0" t="s">
-        <x:v>477</x:v>
-      </x:c>
-      <x:c r="B48" s="0" t="s">
-        <x:v>478</x:v>
-      </x:c>
-      <x:c r="C48" s="2">
-        <x:v>45023.3467592593</x:v>
-      </x:c>
-      <x:c r="D48" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E48" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F48" s="3" t="s">
-        <x:v>479</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="49" spans="1:6">
-      <x:c r="A49" s="0" t="s">
-        <x:v>480</x:v>
-      </x:c>
-      <x:c r="B49" s="0" t="s">
-        <x:v>481</x:v>
-      </x:c>
-      <x:c r="C49" s="2">
-        <x:v>45021.3024884259</x:v>
-      </x:c>
-      <x:c r="D49" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E49" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F49" s="3" t="s">
-        <x:v>482</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="50" spans="1:6">
-      <x:c r="A50" s="0" t="s">
-        <x:v>483</x:v>
-      </x:c>
-      <x:c r="B50" s="0" t="s">
-        <x:v>484</x:v>
-      </x:c>
-      <x:c r="C50" s="2">
-        <x:v>45015.6384606482</x:v>
-      </x:c>
-      <x:c r="D50" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E50" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F50" s="3" t="s">
-        <x:v>485</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="51" spans="1:6">
-      <x:c r="A51" s="0" t="s">
-        <x:v>486</x:v>
-      </x:c>
-      <x:c r="B51" s="0" t="s">
-        <x:v>487</x:v>
-      </x:c>
-      <x:c r="C51" s="2">
-        <x:v>45012.2876851852</x:v>
-      </x:c>
-      <x:c r="D51" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E51" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F51" s="3" t="s">
-        <x:v>488</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="52" spans="1:6">
-      <x:c r="A52" s="0" t="s">
-        <x:v>489</x:v>
-      </x:c>
-      <x:c r="B52" s="0" t="s">
-        <x:v>490</x:v>
-      </x:c>
-      <x:c r="C52" s="2">
-        <x:v>44960.6602430556</x:v>
-      </x:c>
-      <x:c r="D52" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E52" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F52" s="3" t="s">
-        <x:v>491</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="53" spans="1:6">
-      <x:c r="A53" s="0" t="s">
-        <x:v>492</x:v>
-      </x:c>
-      <x:c r="B53" s="0" t="s">
-        <x:v>493</x:v>
-      </x:c>
-      <x:c r="C53" s="2">
-        <x:v>44944.3327662037</x:v>
-      </x:c>
-      <x:c r="D53" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="E53" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F53" s="3" t="s">
-        <x:v>494</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="54" spans="1:6">
-      <x:c r="A54" s="0" t="s">
-        <x:v>495</x:v>
-      </x:c>
-      <x:c r="B54" s="0" t="s">
-        <x:v>496</x:v>
-      </x:c>
-      <x:c r="C54" s="2">
-        <x:v>44867.5149074074</x:v>
-      </x:c>
-      <x:c r="D54" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="E54" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F54" s="3" t="s">
-        <x:v>497</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="55" spans="1:6">
-      <x:c r="A55" s="0" t="s">
-        <x:v>498</x:v>
-      </x:c>
-      <x:c r="B55" s="0" t="s">
-        <x:v>499</x:v>
-      </x:c>
-      <x:c r="C55" s="2">
-        <x:v>44865.3693634259</x:v>
-      </x:c>
-      <x:c r="D55" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E55" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F55" s="3" t="s">
-        <x:v>500</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="56" spans="1:6">
-      <x:c r="A56" s="0" t="s">
-        <x:v>501</x:v>
-      </x:c>
-      <x:c r="B56" s="0" t="s">
-        <x:v>502</x:v>
-      </x:c>
-      <x:c r="C56" s="2">
-        <x:v>44841.842025463</x:v>
-      </x:c>
-      <x:c r="D56" s="0">
-        <x:v>42</x:v>
-      </x:c>
-      <x:c r="E56" s="0">
-        <x:v>40</x:v>
-      </x:c>
-      <x:c r="F56" s="3" t="s">
-        <x:v>503</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="57" spans="1:6">
-      <x:c r="A57" s="0" t="s">
-        <x:v>504</x:v>
-      </x:c>
-      <x:c r="B57" s="0" t="s">
-        <x:v>505</x:v>
-      </x:c>
-      <x:c r="C57" s="2">
-        <x:v>44818.6455555556</x:v>
-      </x:c>
-      <x:c r="D57" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E57" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F57" s="3" t="s">
-        <x:v>506</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="58" spans="1:6">
-      <x:c r="A58" s="0" t="s">
-        <x:v>507</x:v>
-      </x:c>
-      <x:c r="B58" s="0" t="s">
-        <x:v>508</x:v>
-      </x:c>
-      <x:c r="C58" s="2">
-        <x:v>44805.3499884259</x:v>
-      </x:c>
-      <x:c r="D58" s="0">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="E58" s="0">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="F58" s="3" t="s">
-        <x:v>509</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="59" spans="1:6">
-      <x:c r="A59" s="0" t="s">
-        <x:v>510</x:v>
-      </x:c>
-      <x:c r="B59" s="0" t="s">
-        <x:v>511</x:v>
-      </x:c>
-      <x:c r="C59" s="2">
-        <x:v>44796.4331712963</x:v>
-      </x:c>
-      <x:c r="D59" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="E59" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F59" s="3" t="s">
-        <x:v>512</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="60" spans="1:6">
-      <x:c r="A60" s="0" t="s">
-        <x:v>513</x:v>
-      </x:c>
-      <x:c r="B60" s="0" t="s">
-        <x:v>514</x:v>
-      </x:c>
-      <x:c r="C60" s="2">
-        <x:v>44787.841712963</x:v>
-      </x:c>
-      <x:c r="D60" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E60" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F60" s="3" t="s">
-        <x:v>515</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="61" spans="1:6">
-      <x:c r="A61" s="0" t="s">
-        <x:v>516</x:v>
-      </x:c>
-      <x:c r="B61" s="0" t="s">
-        <x:v>517</x:v>
-      </x:c>
-      <x:c r="C61" s="2">
-        <x:v>44693.2737731481</x:v>
-      </x:c>
-      <x:c r="D61" s="0">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="E61" s="0">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="F61" s="3" t="s">
-        <x:v>518</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="62" spans="1:6">
-      <x:c r="A62" s="0" t="s">
-        <x:v>519</x:v>
-      </x:c>
-      <x:c r="B62" s="0" t="s">
-        <x:v>520</x:v>
-      </x:c>
-      <x:c r="C62" s="2">
-        <x:v>44602.6183680556</x:v>
-      </x:c>
-      <x:c r="D62" s="0">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="E62" s="0">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="F62" s="3" t="s">
-        <x:v>521</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="63" spans="1:6">
-      <x:c r="A63" s="0" t="s">
-        <x:v>522</x:v>
-      </x:c>
-      <x:c r="B63" s="0" t="s">
-        <x:v>523</x:v>
-      </x:c>
-      <x:c r="C63" s="2">
-        <x:v>44557.8673263889</x:v>
-      </x:c>
-      <x:c r="D63" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E63" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F63" s="3" t="s">
-        <x:v>524</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="64" spans="1:6">
-      <x:c r="A64" s="0" t="s">
-        <x:v>525</x:v>
-      </x:c>
-      <x:c r="B64" s="0" t="s">
-        <x:v>526</x:v>
-      </x:c>
-      <x:c r="C64" s="2">
-        <x:v>44460.5544907407</x:v>
-      </x:c>
-      <x:c r="D64" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="E64" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F64" s="3" t="s">
-        <x:v>527</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="65" spans="1:6">
-      <x:c r="A65" s="0" t="s">
-        <x:v>528</x:v>
-      </x:c>
-      <x:c r="B65" s="0" t="s">
-        <x:v>529</x:v>
-      </x:c>
-      <x:c r="C65" s="2">
-        <x:v>44455.7410416667</x:v>
-      </x:c>
-      <x:c r="D65" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E65" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F65" s="3" t="s">
-        <x:v>530</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="66" spans="1:6">
-      <x:c r="A66" s="0" t="s">
-        <x:v>531</x:v>
-      </x:c>
-      <x:c r="B66" s="0" t="s">
-        <x:v>532</x:v>
-      </x:c>
-      <x:c r="C66" s="2">
-        <x:v>44441.8997800926</x:v>
-      </x:c>
-      <x:c r="D66" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E66" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F66" s="3" t="s">
-        <x:v>533</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="67" spans="1:6">
-      <x:c r="A67" s="0" t="s">
-        <x:v>534</x:v>
-      </x:c>
-      <x:c r="B67" s="0" t="s">
-        <x:v>535</x:v>
-      </x:c>
-      <x:c r="C67" s="2">
-        <x:v>44385.8234722222</x:v>
-      </x:c>
-      <x:c r="D67" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E67" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F67" s="3" t="s">
-        <x:v>536</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="68" spans="1:6">
-      <x:c r="A68" s="0" t="s">
-        <x:v>537</x:v>
-      </x:c>
-      <x:c r="B68" s="0" t="s">
-        <x:v>538</x:v>
-      </x:c>
-      <x:c r="C68" s="2">
-        <x:v>44377.8052893519</x:v>
-      </x:c>
-      <x:c r="D68" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E68" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F68" s="3" t="s">
-        <x:v>539</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="69" spans="1:6">
-      <x:c r="A69" s="0" t="s">
-        <x:v>540</x:v>
-      </x:c>
-      <x:c r="B69" s="0" t="s">
-        <x:v>541</x:v>
-      </x:c>
-      <x:c r="C69" s="2">
-        <x:v>44368.9983217593</x:v>
-      </x:c>
-      <x:c r="D69" s="0">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="E69" s="0">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="F69" s="3" t="s">
-        <x:v>542</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="70" spans="1:6">
-      <x:c r="A70" s="0" t="s">
-        <x:v>543</x:v>
-      </x:c>
-      <x:c r="B70" s="0" t="s">
-        <x:v>544</x:v>
-      </x:c>
-      <x:c r="C70" s="2">
-        <x:v>44357.5082175926</x:v>
-      </x:c>
-      <x:c r="D70" s="0">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="E70" s="0">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="F70" s="3" t="s">
-        <x:v>545</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="71" spans="1:6">
-      <x:c r="A71" s="0" t="s">
-        <x:v>546</x:v>
-      </x:c>
-      <x:c r="B71" s="0" t="s">
-        <x:v>547</x:v>
-      </x:c>
-      <x:c r="C71" s="2">
-        <x:v>44356.9047106481</x:v>
-      </x:c>
-      <x:c r="D71" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E71" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F71" s="3" t="s">
-        <x:v>548</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="72" spans="1:6">
-      <x:c r="A72" s="0" t="s">
-        <x:v>549</x:v>
-      </x:c>
-      <x:c r="B72" s="0" t="s">
-        <x:v>550</x:v>
-      </x:c>
-      <x:c r="C72" s="2">
-        <x:v>44328.1607986111</x:v>
-      </x:c>
-      <x:c r="D72" s="0">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="E72" s="0">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="F72" s="3" t="s">
-        <x:v>551</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="73" spans="1:6">
-      <x:c r="A73" s="0" t="s">
-        <x:v>552</x:v>
-      </x:c>
-      <x:c r="B73" s="0" t="s">
-        <x:v>553</x:v>
-      </x:c>
-      <x:c r="C73" s="2">
-        <x:v>44326.8594212963</x:v>
-      </x:c>
-      <x:c r="D73" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E73" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F73" s="3" t="s">
-        <x:v>554</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="74" spans="1:6">
-      <x:c r="A74" s="0" t="s">
-        <x:v>555</x:v>
-      </x:c>
-      <x:c r="B74" s="0" t="s">
-        <x:v>556</x:v>
-      </x:c>
-      <x:c r="C74" s="2">
-        <x:v>44307.2285416667</x:v>
-      </x:c>
-      <x:c r="D74" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E74" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F74" s="3" t="s">
-        <x:v>557</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="75" spans="1:6">
-      <x:c r="A75" s="0" t="s">
-        <x:v>558</x:v>
-      </x:c>
-      <x:c r="B75" s="0" t="s">
-        <x:v>559</x:v>
-      </x:c>
-      <x:c r="C75" s="2">
-        <x:v>44285.6562962963</x:v>
-      </x:c>
-      <x:c r="D75" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E75" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F75" s="3" t="s">
-        <x:v>560</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="76" spans="1:6">
-      <x:c r="A76" s="0" t="s">
-        <x:v>561</x:v>
-      </x:c>
-      <x:c r="B76" s="0" t="s">
-        <x:v>562</x:v>
-      </x:c>
-      <x:c r="C76" s="2">
-        <x:v>44264.9472222222</x:v>
-      </x:c>
-      <x:c r="D76" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E76" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F76" s="0" t="s">
-        <x:v>563</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="77" spans="1:6">
-      <x:c r="A77" s="0" t="s">
-        <x:v>564</x:v>
-      </x:c>
-      <x:c r="B77" s="0" t="s">
-        <x:v>565</x:v>
-      </x:c>
-      <x:c r="C77" s="2">
-        <x:v>44210.6206365741</x:v>
-      </x:c>
-      <x:c r="D77" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E77" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F77" s="3" t="s">
-        <x:v>566</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="78" spans="1:6">
-      <x:c r="A78" s="0" t="s">
-        <x:v>567</x:v>
-      </x:c>
-      <x:c r="B78" s="0" t="s">
-        <x:v>568</x:v>
-      </x:c>
-      <x:c r="C78" s="2">
-        <x:v>44180.6690972222</x:v>
-      </x:c>
-      <x:c r="D78" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E78" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F78" s="3" t="s">
-        <x:v>569</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="79" spans="1:6">
-      <x:c r="A79" s="0" t="s">
-        <x:v>570</x:v>
-      </x:c>
-      <x:c r="B79" s="0" t="s">
-        <x:v>571</x:v>
-      </x:c>
-      <x:c r="C79" s="2">
-        <x:v>44134.7731134259</x:v>
-      </x:c>
-      <x:c r="D79" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E79" s="0">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="80" spans="1:6">
-      <x:c r="A80" s="0" t="s">
-        <x:v>572</x:v>
-      </x:c>
-      <x:c r="B80" s="0" t="s">
-        <x:v>573</x:v>
-      </x:c>
-      <x:c r="C80" s="2">
-        <x:v>44085.8156828704</x:v>
-      </x:c>
-      <x:c r="D80" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E80" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F80" s="3" t="s">
-        <x:v>574</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="81" spans="1:6">
-      <x:c r="A81" s="0" t="s">
-        <x:v>575</x:v>
-      </x:c>
-      <x:c r="B81" s="0" t="s">
-        <x:v>576</x:v>
-      </x:c>
-      <x:c r="C81" s="2">
-        <x:v>44049.0976388889</x:v>
-      </x:c>
-      <x:c r="D81" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E81" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F81" s="3" t="s">
-        <x:v>577</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="82" spans="1:6">
-      <x:c r="A82" s="0" t="s">
-        <x:v>578</x:v>
-      </x:c>
-      <x:c r="B82" s="0" t="s">
-        <x:v>579</x:v>
-      </x:c>
-      <x:c r="C82" s="2">
-        <x:v>44028.3084027778</x:v>
-      </x:c>
-      <x:c r="D82" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E82" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F82" s="3" t="s">
-        <x:v>580</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="83" spans="1:6">
-      <x:c r="A83" s="0" t="s">
-        <x:v>581</x:v>
-      </x:c>
-      <x:c r="B83" s="0" t="s">
-        <x:v>582</x:v>
-      </x:c>
-      <x:c r="C83" s="2">
-        <x:v>44011.4896296296</x:v>
-      </x:c>
-      <x:c r="D83" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E83" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F83" s="3" t="s">
-        <x:v>583</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="84" spans="1:6">
-      <x:c r="A84" s="0" t="s">
-        <x:v>584</x:v>
-      </x:c>
-      <x:c r="B84" s="0" t="s">
-        <x:v>585</x:v>
-      </x:c>
-      <x:c r="C84" s="2">
-        <x:v>43968.691875</x:v>
-      </x:c>
-      <x:c r="D84" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E84" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F84" s="3" t="s">
-        <x:v>586</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="85" spans="1:6">
-      <x:c r="A85" s="0" t="s">
-        <x:v>587</x:v>
-      </x:c>
-      <x:c r="B85" s="0" t="s">
-        <x:v>588</x:v>
-      </x:c>
-      <x:c r="C85" s="2">
-        <x:v>43956.5750694444</x:v>
-      </x:c>
-      <x:c r="D85" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="E85" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F85" s="3" t="s">
-        <x:v>589</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="86" spans="1:6">
-      <x:c r="A86" s="0" t="s">
-        <x:v>590</x:v>
-      </x:c>
-      <x:c r="B86" s="0" t="s">
-        <x:v>591</x:v>
-      </x:c>
-      <x:c r="C86" s="2">
-        <x:v>43938.6813078704</x:v>
-      </x:c>
-      <x:c r="D86" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E86" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F86" s="3" t="s">
-        <x:v>592</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="87" spans="1:6">
-      <x:c r="A87" s="0" t="s">
-        <x:v>593</x:v>
-      </x:c>
-      <x:c r="B87" s="0" t="s">
-        <x:v>594</x:v>
-      </x:c>
-      <x:c r="C87" s="2">
-        <x:v>43938.64375</x:v>
-      </x:c>
-      <x:c r="D87" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E87" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F87" s="3" t="s">
-        <x:v>595</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="88" spans="1:6">
-      <x:c r="A88" s="0" t="s">
-        <x:v>596</x:v>
-      </x:c>
-      <x:c r="B88" s="0" t="s">
-        <x:v>597</x:v>
-      </x:c>
-      <x:c r="C88" s="2">
-        <x:v>43916.6301157407</x:v>
-      </x:c>
-      <x:c r="D88" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="E88" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F88" s="3" t="s">
-        <x:v>598</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="89" spans="1:6">
-      <x:c r="A89" s="0" t="s">
-        <x:v>599</x:v>
-      </x:c>
-      <x:c r="B89" s="0" t="s">
-        <x:v>600</x:v>
-      </x:c>
-      <x:c r="C89" s="2">
-        <x:v>43903.5819328704</x:v>
-      </x:c>
-      <x:c r="D89" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="E89" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F89" s="3" t="s">
-        <x:v>601</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="90" spans="1:6">
-      <x:c r="A90" s="0" t="s">
-        <x:v>602</x:v>
-      </x:c>
-      <x:c r="B90" s="0" t="s">
-        <x:v>603</x:v>
-      </x:c>
-      <x:c r="C90" s="2">
-        <x:v>43902.6278356481</x:v>
-      </x:c>
-      <x:c r="D90" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E90" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F90" s="3" t="s">
-        <x:v>604</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="91" spans="1:6">
-      <x:c r="A91" s="0" t="s">
-        <x:v>605</x:v>
-      </x:c>
-      <x:c r="B91" s="0" t="s">
-        <x:v>606</x:v>
-      </x:c>
-      <x:c r="C91" s="2">
-        <x:v>43818.8870717593</x:v>
-      </x:c>
-      <x:c r="D91" s="0">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E91" s="0">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="F91" s="3" t="s">
-        <x:v>607</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="92" spans="1:6">
-      <x:c r="A92" s="0" t="s">
-        <x:v>608</x:v>
-      </x:c>
-      <x:c r="B92" s="0" t="s">
-        <x:v>609</x:v>
-      </x:c>
-      <x:c r="C92" s="2">
-        <x:v>43810.5890393518</x:v>
-      </x:c>
-      <x:c r="D92" s="0">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E92" s="0">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="F92" s="3" t="s">
-        <x:v>610</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="93" spans="1:6">
-      <x:c r="A93" s="0" t="s">
-        <x:v>611</x:v>
-      </x:c>
-      <x:c r="B93" s="0" t="s">
-        <x:v>612</x:v>
-      </x:c>
-      <x:c r="C93" s="2">
-        <x:v>43810.5550810185</x:v>
-      </x:c>
-      <x:c r="D93" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="E93" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F93" s="0" t="s">
-        <x:v>613</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="94" spans="1:6">
-      <x:c r="A94" s="0" t="s">
-        <x:v>614</x:v>
-      </x:c>
-      <x:c r="B94" s="0" t="s">
-        <x:v>615</x:v>
-      </x:c>
-      <x:c r="C94" s="2">
-        <x:v>43810.5538657407</x:v>
-      </x:c>
-      <x:c r="D94" s="0">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="E94" s="0">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="F94" s="0" t="s">
-        <x:v>616</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="95" spans="1:6">
-      <x:c r="A95" s="0" t="s">
-        <x:v>617</x:v>
-      </x:c>
-      <x:c r="B95" s="0" t="s">
-        <x:v>618</x:v>
-      </x:c>
-      <x:c r="C95" s="2">
-        <x:v>43810.552662037</x:v>
-      </x:c>
-      <x:c r="D95" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="E95" s="0">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F95" s="3" t="s">
-        <x:v>619</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="96" spans="1:6">
-      <x:c r="A96" s="0" t="s">
-        <x:v>620</x:v>
-      </x:c>
-      <x:c r="B96" s="0" t="s">
-        <x:v>621</x:v>
-      </x:c>
-      <x:c r="C96" s="2">
-        <x:v>43810.5428587963</x:v>
-      </x:c>
-      <x:c r="D96" s="0">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="E96" s="0">
-        <x:v>46</x:v>
-      </x:c>
-      <x:c r="F96" s="0" t="s">
-        <x:v>622</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -9895,11 +6744,11 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="35.710625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="44.210625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="14.960625" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="9.210625" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="15.960625" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="41.424911" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="47.282054" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="15.282054" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="9.567768" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="16.567768" style="0" customWidth="1"/>
     <x:col min="6" max="6" width="255" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
@@ -9925,10 +6774,10 @@
     </x:row>
     <x:row r="2" spans="1:6">
       <x:c r="A2" s="0" t="s">
-        <x:v>623</x:v>
+        <x:v>440</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>624</x:v>
+        <x:v>441</x:v>
       </x:c>
       <x:c r="C2" s="2">
         <x:v>45377.6785069444</x:v>
@@ -9940,15 +6789,15 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="F2" s="0" t="s">
-        <x:v>625</x:v>
+        <x:v>442</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:6">
       <x:c r="A3" s="0" t="s">
-        <x:v>626</x:v>
+        <x:v>443</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>627</x:v>
+        <x:v>444</x:v>
       </x:c>
       <x:c r="C3" s="2">
         <x:v>45377.6762037037</x:v>
@@ -9960,7 +6809,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="F3" s="0" t="s">
-        <x:v>628</x:v>
+        <x:v>445</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>